<commit_message>
Articulation Test by age (v1)
</commit_message>
<xml_diff>
--- a/Doc/articulation_test_eng_v2.xlsx
+++ b/Doc/articulation_test_eng_v2.xlsx
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ENG_SQL!$A$1:$E$81</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ENG_SQL (2)'!$B$1:$G$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ENG_SQL (2)'!$A$1:$I$86</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="276">
   <si>
     <t>Sounds</t>
   </si>
@@ -791,20 +791,83 @@
     <t>thvl</t>
   </si>
   <si>
-    <t>tho</t>
-  </si>
-  <si>
     <t>sound order</t>
   </si>
   <si>
     <t>position order</t>
+  </si>
+  <si>
+    <t>chips</t>
+  </si>
+  <si>
+    <t>mummy</t>
+  </si>
+  <si>
+    <t>cannon</t>
+  </si>
+  <si>
+    <t>hardhat</t>
+  </si>
+  <si>
+    <t>pepper</t>
+  </si>
+  <si>
+    <t>baby</t>
+  </si>
+  <si>
+    <t>tent</t>
+  </si>
+  <si>
+    <t>cockerel</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>daddy</t>
+  </si>
+  <si>
+    <t>goggles</t>
+  </si>
+  <si>
+    <t>fifteen</t>
+  </si>
+  <si>
+    <t>swinging</t>
+  </si>
+  <si>
+    <t>lollipop</t>
+  </si>
+  <si>
+    <t>buses</t>
+  </si>
+  <si>
+    <t>yoyo</t>
+  </si>
+  <si>
+    <t>church</t>
+  </si>
+  <si>
+    <t>robber</t>
+  </si>
+  <si>
+    <t>george</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,6 +925,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -949,7 +1020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1009,6 +1080,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1766,1724 +1852,2643 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H86" sqref="H2:H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="7.26953125" customWidth="1"/>
-    <col min="6" max="6" width="27.54296875" customWidth="1"/>
-    <col min="7" max="7" width="78" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="35" customFormat="1" ht="29">
+      <c r="A1" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="E1" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>254</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="I1" s="38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="19">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="19">
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="str">
+        <f>E2&amp;".jpg"</f>
+        <v>mole.jpg</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D2,"','",E2,"','",F2,"','",G2,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mole','Initial','mole.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" s="33">
+        <v>2</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" t="str">
+        <f>E3&amp;".jpg"</f>
+        <v>drum.jpg</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D3,"','",E3,"','",F3,"','",G3,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','drum','Final','drum.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26">
+        <v>3</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="str">
+        <f>E4&amp;".jpg"</f>
+        <v>lemon.jpg</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D4,"','",E4,"','",F4,"','",G4,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','lemon','Medial','lemon.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" t="s">
         <v>83</v>
       </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F33" si="0">C2&amp;".jpg"</f>
-        <v>mole.jpg</v>
-      </c>
-      <c r="G2" t="str">
-        <f t="shared" ref="G2:G33" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",B2,"','",C2,"','",E2,"','",F2,"', 'EN');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mole','Initial','mole.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+      <c r="G5" t="str">
+        <f>E5&amp;".jpg"</f>
+        <v>pen.jpg</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D5,"','",E5,"','",F5,"','",G5,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','pen','Initial','pen.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="33">
+        <v>2</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" t="str">
+        <f>E6&amp;".jpg"</f>
+        <v>map.jpg</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D6,"','",E6,"','",F6,"','",G6,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','map','Final','map.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="26">
+        <v>3</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" t="str">
+        <f>E7&amp;".jpg"</f>
+        <v>teapot.jpg</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D7,"','",E7,"','",F7,"','",G7,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','teapot','Medial','teapot.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="D8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" t="str">
+        <f>E8&amp;".jpg"</f>
+        <v>hen.jpg</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D8,"','",E8,"','",F8,"','",G8,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hen','Initial','hen.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" t="str">
+        <f>E9&amp;".jpg"</f>
+        <v>boot.jpg</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D9,"','",E9,"','",F9,"','",G9,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','boot','Initial','boot.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="33">
+        <v>2</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" t="str">
+        <f>E10&amp;".jpg"</f>
+        <v>cub.jpg</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D10,"','",E10,"','",F10,"','",G10,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','cub','Final','cub.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="26">
+        <v>3</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" t="str">
+        <f>E11&amp;".jpg"</f>
+        <v>robot.jpg</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D11,"','",E11,"','",F11,"','",G11,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','robot','Medial','robot.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
         <v>5</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="D3" s="33">
+      <c r="C12" s="19">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" t="str">
+        <f>E12&amp;".jpg"</f>
+        <v>wolf.jpg</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D12,"','",E12,"','",F12,"','",G12,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','wolf','Initial','wolf.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" s="33">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D13" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
         <v>85</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>drum.jpg</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','drum','Final','drum.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="G13" t="str">
+        <f>E13&amp;".jpg"</f>
+        <v>cow.jpg</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D13,"','",E13,"','",F13,"','",G13,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','cow','Final','cow.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" s="26">
+        <v>3</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="str">
+        <f>E14&amp;".jpg"</f>
+        <v>tower.jpg</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D14,"','",E14,"','",F14,"','",G14,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','tower','Medial','tower.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" s="19">
         <v>1</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="D15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" t="str">
+        <f>E15&amp;".jpg"</f>
+        <v>train.jpg</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D15,"','",E15,"','",F15,"','",G15,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','train','Initial','train.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" s="33">
+        <v>2</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="str">
+        <f>E16&amp;".jpg"</f>
+        <v>hat.jpg</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D16,"','",E16,"','",F16,"','",G16,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','hat','Final','hat.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" s="26">
+        <v>3</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" t="str">
+        <f>E17&amp;".jpg"</f>
+        <v>water.jpg</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D17,"','",E17,"','",F17,"','",G17,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','water','Medial','water.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" s="19">
+        <v>1</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" t="str">
+        <f>E18&amp;".jpg"</f>
+        <v>cat.jpg</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D18,"','",E18,"','",F18,"','",G18,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','cat','Initial','cat.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" s="33">
+        <v>2</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" t="str">
+        <f>E19&amp;".jpg"</f>
+        <v>sock.jpg</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D19,"','",E19,"','",F19,"','",G19,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','sock','Final','sock.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" s="26">
+        <v>3</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" t="str">
+        <f>E20&amp;".jpg"</f>
+        <v>rocket.jpg</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D20,"','",E20,"','",F20,"','",G20,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','rocket','Medial','rocket.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" s="19">
+        <v>1</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" t="str">
+        <f>E21&amp;".jpg"</f>
+        <v>gate.jpg</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D21,"','",E21,"','",F21,"','",G21,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gate','Initial','gate.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22" s="33">
+        <v>2</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" t="str">
+        <f>E22&amp;".jpg"</f>
+        <v>bag.jpg</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D22,"','",E22,"','",F22,"','",G22,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','bag','Final','bag.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" s="26">
+        <v>3</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" t="str">
+        <f>E23&amp;".jpg"</f>
+        <v>tiger.jpg</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D23,"','",E23,"','",F23,"','",G23,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','tiger','Medial','tiger.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="F24" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" t="str">
+        <f>E24&amp;".jpg"</f>
+        <v>fan.jpg</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D24,"','",E24,"','",F24,"','",G24,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fan','Initial','fan.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25" s="33">
+        <v>2</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" t="str">
+        <f>E25&amp;".jpg"</f>
+        <v>laugh.jpg</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D25,"','",E25,"','",F25,"','",G25,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','laugh','Final','laugh.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26" s="26">
+        <v>3</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" t="str">
+        <f>E26&amp;".jpg"</f>
+        <v>wafer.jpg</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D26,"','",E26,"','",F26,"','",G26,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','wafer','Medial','wafer.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27" s="19">
+        <v>1</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" t="str">
+        <f>E27&amp;".jpg"</f>
+        <v>dog.jpg</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D27,"','",E27,"','",F27,"','",G27,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','dog','Initial','dog.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28" s="33">
+        <v>2</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" t="str">
+        <f>E28&amp;".jpg"</f>
+        <v>head.jpg</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D28,"','",E28,"','",F28,"','",G28,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','head','Final','head.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29" s="26">
+        <v>3</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" t="str">
+        <f>E29&amp;".jpg"</f>
+        <v>puddle.jpg</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D29,"','",E29,"','",F29,"','",G29,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','puddle','Medial','puddle.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" t="str">
+        <f>E30&amp;".jpg"</f>
+        <v>nut.jpg</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D30,"','",E30,"','",F30,"','",G30,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','nut','Initial','nut.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="C31" s="33">
+        <v>2</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="str">
+        <f>E31&amp;".jpg"</f>
+        <v>pin.jpg</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D31,"','",E31,"','",F31,"','",G31,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','pin','Final','pin.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>11</v>
+      </c>
+      <c r="C32" s="26">
+        <v>3</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" t="str">
+        <f>E32&amp;".jpg"</f>
+        <v>dinner.jpg</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D32,"','",E32,"','",F32,"','",G32,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','dinner','Medial','dinner.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33" s="33">
+        <v>2</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" t="str">
+        <f>E33&amp;".jpg"</f>
+        <v>wing.jpg</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D33,"','",E33,"','",F33,"','",G33,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','wing','Final','wing.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34" s="26">
+        <v>3</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" t="s">
+        <v>84</v>
+      </c>
+      <c r="G34" t="str">
+        <f>E34&amp;".jpg"</f>
+        <v>finger.jpg</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D34,"','",E34,"','",F34,"','",G34,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','finger','Medial','finger.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" t="str">
+        <f>E35&amp;".jpg"</f>
+        <v>yak.jpg</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D35,"','",E35,"','",F35,"','",G35,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yak','Initial','yak.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>13</v>
+      </c>
+      <c r="C36" s="33">
+        <v>2</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="F36" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" t="str">
+        <f>E36&amp;".jpg"</f>
+        <v>boy.jpg</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D36,"','",E36,"','",F36,"','",G36,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','boy','Final','boy.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>13</v>
+      </c>
+      <c r="C37" s="26">
+        <v>3</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" t="s">
+        <v>84</v>
+      </c>
+      <c r="G37" t="str">
+        <f>E37&amp;".jpg"</f>
+        <v>crayon.jpg</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D37,"','",E37,"','",F37,"','",G37,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','crayon','Medial','crayon.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>14</v>
+      </c>
+      <c r="C38" s="19">
+        <v>1</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" t="str">
+        <f>E38&amp;".jpg"</f>
+        <v>sun.jpg</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D38,"','",E38,"','",F38,"','",G38,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','sun','Initial','sun.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>14</v>
+      </c>
+      <c r="C39" s="33">
+        <v>2</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F39" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" t="str">
+        <f>E39&amp;".jpg"</f>
+        <v>mouse.jpg</v>
+      </c>
+      <c r="H39">
+        <v>6</v>
+      </c>
+      <c r="I39" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D39,"','",E39,"','",F39,"','",G39,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','mouse','Final','mouse.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40" s="26">
+        <v>3</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F40" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" t="str">
+        <f>E40&amp;".jpg"</f>
+        <v>listen.jpg</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D40,"','",E40,"','",F40,"','",G40,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','listen','Medial','listen.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>15</v>
+      </c>
+      <c r="C41" s="19">
+        <v>1</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G41" t="str">
+        <f>E41&amp;".jpg"</f>
+        <v>shower.jpg</v>
+      </c>
+      <c r="H41">
+        <v>6</v>
+      </c>
+      <c r="I41" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D41,"','",E41,"','",F41,"','",G41,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','shower','Initial','shower.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>15</v>
+      </c>
+      <c r="C42" s="33">
+        <v>2</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" t="str">
+        <f>E42&amp;".jpg"</f>
+        <v>fish.jpg</v>
+      </c>
+      <c r="H42">
+        <v>6</v>
+      </c>
+      <c r="I42" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D42,"','",E42,"','",F42,"','",G42,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','fish','Final','fish.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>15</v>
+      </c>
+      <c r="C43" s="26">
+        <v>3</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F43" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" t="str">
+        <f>E43&amp;".jpg"</f>
+        <v>mushroom.jpg</v>
+      </c>
+      <c r="H43">
+        <v>6</v>
+      </c>
+      <c r="I43" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D43,"','",E43,"','",F43,"','",G43,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','mushroom','Medial','mushroom.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>16</v>
+      </c>
+      <c r="C44" s="19">
+        <v>1</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="F44" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" t="str">
+        <f>E44&amp;".jpg"</f>
+        <v>zip.jpg</v>
+      </c>
+      <c r="H44">
+        <v>6</v>
+      </c>
+      <c r="I44" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D44,"','",E44,"','",F44,"','",G44,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','zip','Initial','zip.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>16</v>
+      </c>
+      <c r="C45" s="33">
+        <v>2</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="F45" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" t="str">
+        <f>E45&amp;".jpg"</f>
+        <v>bees.jpg</v>
+      </c>
+      <c r="H45">
+        <v>6</v>
+      </c>
+      <c r="I45" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D45,"','",E45,"','",F45,"','",G45,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','bees','Final','bees.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46" s="26">
+        <v>3</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="F46" t="s">
+        <v>84</v>
+      </c>
+      <c r="G46" t="str">
+        <f>E46&amp;".jpg"</f>
+        <v>puzzle.jpg</v>
+      </c>
+      <c r="H46">
+        <v>6</v>
+      </c>
+      <c r="I46" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D46,"','",E46,"','",F46,"','",G46,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','puzzle','Medial','puzzle.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>17</v>
+      </c>
+      <c r="C47" s="19">
+        <v>1</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" t="s">
+        <v>83</v>
+      </c>
+      <c r="G47" t="str">
+        <f>E47&amp;".jpg"</f>
+        <v>log.jpg</v>
+      </c>
+      <c r="H47">
+        <v>6</v>
+      </c>
+      <c r="I47" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D47,"','",E47,"','",F47,"','",G47,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','log','Initial','log.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>17</v>
+      </c>
+      <c r="C48" s="33">
+        <v>2</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" t="str">
+        <f>E48&amp;".jpg"</f>
+        <v>hill.jpg</v>
+      </c>
+      <c r="H48">
+        <v>6</v>
+      </c>
+      <c r="I48" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D48,"','",E48,"','",F48,"','",G48,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','hill','Final','hill.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>17</v>
+      </c>
+      <c r="C49" s="26">
+        <v>3</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" t="s">
+        <v>84</v>
+      </c>
+      <c r="G49" t="str">
+        <f>E49&amp;".jpg"</f>
+        <v>tulip.jpg</v>
+      </c>
+      <c r="H49">
+        <v>6</v>
+      </c>
+      <c r="I49" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D49,"','",E49,"','",F49,"','",G49,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','tulip','Medial','tulip.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>18</v>
+      </c>
+      <c r="C50" s="19">
+        <v>1</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F50" t="s">
+        <v>83</v>
+      </c>
+      <c r="G50" t="str">
+        <f>E50&amp;".jpg"</f>
+        <v>van.jpg</v>
+      </c>
+      <c r="H50">
+        <v>6</v>
+      </c>
+      <c r="I50" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D50,"','",E50,"','",F50,"','",G50,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','van','Initial','van.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>18</v>
+      </c>
+      <c r="C51" s="33">
+        <v>2</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" t="s">
+        <v>85</v>
+      </c>
+      <c r="G51" t="str">
+        <f>E51&amp;".jpg"</f>
+        <v>sieve.jpg</v>
+      </c>
+      <c r="H51">
+        <v>6</v>
+      </c>
+      <c r="I51" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D51,"','",E51,"','",F51,"','",G51,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','sieve','Final','sieve.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>18</v>
+      </c>
+      <c r="C52" s="26">
+        <v>3</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F52" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" t="str">
+        <f>E52&amp;".jpg"</f>
+        <v>waving.jpg</v>
+      </c>
+      <c r="H52">
+        <v>6</v>
+      </c>
+      <c r="I52" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D52,"','",E52,"','",F52,"','",G52,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','waving','Medial','waving.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>19</v>
+      </c>
+      <c r="C53" s="19">
+        <v>1</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F53" t="s">
+        <v>83</v>
+      </c>
+      <c r="G53" t="str">
+        <f>E53&amp;".jpg"</f>
+        <v>jam.jpg</v>
+      </c>
+      <c r="H53">
+        <v>7</v>
+      </c>
+      <c r="I53" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D53,"','",E53,"','",F53,"','",G53,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','jam','Initial','jam.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>19</v>
+      </c>
+      <c r="C54" s="33">
+        <v>2</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" t="s">
+        <v>85</v>
+      </c>
+      <c r="G54" t="str">
+        <f>E54&amp;".jpg"</f>
+        <v>midge.jpg</v>
+      </c>
+      <c r="H54">
+        <v>7</v>
+      </c>
+      <c r="I54" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D54,"','",E54,"','",F54,"','",G54,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','midge','Final','midge.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>19</v>
+      </c>
+      <c r="C55" s="26">
+        <v>3</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F55" t="s">
+        <v>84</v>
+      </c>
+      <c r="G55" t="str">
+        <f>E55&amp;".jpg"</f>
+        <v>badger.jpg</v>
+      </c>
+      <c r="H55">
+        <v>7</v>
+      </c>
+      <c r="I55" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D55,"','",E55,"','",F55,"','",G55,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','badger','Medial','badger.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>20</v>
+      </c>
+      <c r="C56" s="19">
+        <v>1</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="F56" t="s">
+        <v>83</v>
+      </c>
+      <c r="G56" t="str">
+        <f>E56&amp;".jpg"</f>
+        <v>chips.jpg</v>
+      </c>
+      <c r="H56">
+        <v>7</v>
+      </c>
+      <c r="I56" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D56,"','",E56,"','",F56,"','",G56,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','chips','Initial','chips.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>20</v>
+      </c>
+      <c r="C57" s="33">
+        <v>2</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F57" t="s">
+        <v>85</v>
+      </c>
+      <c r="G57" t="str">
+        <f>E57&amp;".jpg"</f>
+        <v>witch.jpg</v>
+      </c>
+      <c r="H57">
+        <v>7</v>
+      </c>
+      <c r="I57" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D57,"','",E57,"','",F57,"','",G57,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','witch','Final','witch.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>20</v>
+      </c>
+      <c r="C58" s="26">
+        <v>3</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F58" t="s">
+        <v>84</v>
+      </c>
+      <c r="G58" t="str">
+        <f>E58&amp;".jpg"</f>
+        <v>archer.jpg</v>
+      </c>
+      <c r="H58">
+        <v>7</v>
+      </c>
+      <c r="I58" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D58,"','",E58,"','",F58,"','",G58,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','archer','Medial','archer.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>21</v>
+      </c>
+      <c r="C59" s="19">
+        <v>1</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="F59" t="s">
+        <v>83</v>
+      </c>
+      <c r="G59" t="str">
+        <f>E59&amp;".jpg"</f>
+        <v>thorn.jpg</v>
+      </c>
+      <c r="H59">
+        <v>7</v>
+      </c>
+      <c r="I59" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D59,"','",E59,"','",F59,"','",G59,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','thorn','Initial','thorn.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>21</v>
+      </c>
+      <c r="C60" s="33">
+        <v>2</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" t="s">
+        <v>85</v>
+      </c>
+      <c r="G60" t="str">
+        <f>E60&amp;".jpg"</f>
+        <v>path.jpg</v>
+      </c>
+      <c r="H60">
+        <v>7</v>
+      </c>
+      <c r="I60" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D60,"','",E60,"','",F60,"','",G60,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','path','Final','path.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>21</v>
+      </c>
+      <c r="C61" s="26">
+        <v>3</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="F61" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" t="str">
+        <f>E61&amp;".jpg"</f>
+        <v>birthday.jpg</v>
+      </c>
+      <c r="H61">
+        <v>7</v>
+      </c>
+      <c r="I61" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D61,"','",E61,"','",F61,"','",G61,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','birthday','Medial','birthday.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>22</v>
+      </c>
+      <c r="C62" s="19">
+        <v>1</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="F62" t="s">
+        <v>83</v>
+      </c>
+      <c r="G62" t="str">
+        <f>E62&amp;".jpg"</f>
+        <v>them.jpg</v>
+      </c>
+      <c r="H62">
+        <v>7</v>
+      </c>
+      <c r="I62" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D62,"','",E62,"','",F62,"','",G62,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','them','Initial','them.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>22</v>
+      </c>
+      <c r="C63" s="33">
+        <v>2</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="F63" t="s">
+        <v>85</v>
+      </c>
+      <c r="G63" t="str">
+        <f>E63&amp;".jpg"</f>
+        <v>bathe.jpg</v>
+      </c>
+      <c r="H63">
+        <v>7</v>
+      </c>
+      <c r="I63" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D63,"','",E63,"','",F63,"','",G63,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','bathe','Final','bathe.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>22</v>
+      </c>
+      <c r="C64" s="26">
+        <v>3</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" t="s">
+        <v>84</v>
+      </c>
+      <c r="G64" t="str">
+        <f>E64&amp;".jpg"</f>
+        <v>father.jpg</v>
+      </c>
+      <c r="H64">
+        <v>7</v>
+      </c>
+      <c r="I64" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D64,"','",E64,"','",F64,"','",G64,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','father','Medial','father.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>23</v>
+      </c>
+      <c r="C65" s="26">
+        <v>3</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E65" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="F65" t="s">
+        <v>84</v>
+      </c>
+      <c r="G65" t="str">
+        <f>E65&amp;".jpg"</f>
+        <v>measure.jpg</v>
+      </c>
+      <c r="H65">
+        <v>8</v>
+      </c>
+      <c r="I65" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D65,"','",E65,"','",F65,"','",G65,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('zh','measure','Medial','measure.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>24</v>
+      </c>
+      <c r="C66" s="19">
+        <v>1</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F66" t="s">
+        <v>83</v>
+      </c>
+      <c r="G66" t="str">
+        <f>E66&amp;".jpg"</f>
+        <v>rat.jpg</v>
+      </c>
+      <c r="H66">
+        <v>8</v>
+      </c>
+      <c r="I66" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D66,"','",E66,"','",F66,"','",G66,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','rat','Initial','rat.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>24</v>
+      </c>
+      <c r="C67" s="33">
+        <v>2</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F67" t="s">
+        <v>85</v>
+      </c>
+      <c r="G67" t="str">
+        <f>E67&amp;".jpg"</f>
+        <v>car.jpg</v>
+      </c>
+      <c r="H67">
+        <v>8</v>
+      </c>
+      <c r="I67" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D67,"','",E67,"','",F67,"','",G67,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','car','Final','car.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>24</v>
+      </c>
+      <c r="C68" s="26">
+        <v>3</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F68" t="s">
+        <v>84</v>
+      </c>
+      <c r="G68" t="str">
+        <f>E68&amp;".jpg"</f>
+        <v>barrel.jpg</v>
+      </c>
+      <c r="H68">
+        <v>8</v>
+      </c>
+      <c r="I68" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D68,"','",E68,"','",F68,"','",G68,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','barrel','Medial','barrel.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E69" t="s">
+        <v>255</v>
+      </c>
+      <c r="F69" t="s">
+        <v>86</v>
+      </c>
+      <c r="G69" t="str">
+        <f>E69&amp;".jpg"</f>
+        <v>mummy.jpg</v>
+      </c>
+      <c r="H69">
+        <v>3</v>
+      </c>
+      <c r="I69" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D69,"','",E69,"','",F69,"','",G69,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mummy','Blended','mummy.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>256</v>
+      </c>
+      <c r="F70" t="s">
+        <v>86</v>
+      </c>
+      <c r="G70" t="str">
+        <f>E70&amp;".jpg"</f>
+        <v>cannon.jpg</v>
+      </c>
+      <c r="H70">
+        <v>4</v>
+      </c>
+      <c r="I70" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D70,"','",E70,"','",F70,"','",G70,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','cannon','Blended','cannon.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" t="s">
+        <v>257</v>
+      </c>
+      <c r="F71" t="s">
+        <v>86</v>
+      </c>
+      <c r="G71" t="str">
+        <f>E71&amp;".jpg"</f>
+        <v>hardhat.jpg</v>
+      </c>
+      <c r="H71">
+        <v>3</v>
+      </c>
+      <c r="I71" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D71,"','",E71,"','",F71,"','",G71,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hardhat','Blended','hardhat.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" t="s">
+        <v>258</v>
+      </c>
+      <c r="F72" t="s">
+        <v>86</v>
+      </c>
+      <c r="G72" t="str">
+        <f>E72&amp;".jpg"</f>
+        <v>pepper.jpg</v>
+      </c>
+      <c r="H72">
+        <v>3</v>
+      </c>
+      <c r="I72" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D72,"','",E72,"','",F72,"','",G72,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','pepper','Blended','pepper.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" t="s">
+        <v>259</v>
+      </c>
+      <c r="F73" t="s">
+        <v>86</v>
+      </c>
+      <c r="G73" t="str">
+        <f>E73&amp;".jpg"</f>
+        <v>baby.jpg</v>
+      </c>
+      <c r="H73">
+        <v>3</v>
+      </c>
+      <c r="I73" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D73,"','",E73,"','",F73,"','",G73,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','baby','Blended','baby.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" t="s">
+        <v>260</v>
+      </c>
+      <c r="F74" t="s">
+        <v>86</v>
+      </c>
+      <c r="G74" t="str">
+        <f>E74&amp;".jpg"</f>
+        <v>tent.jpg</v>
+      </c>
+      <c r="H74">
+        <v>4</v>
+      </c>
+      <c r="I74" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D74,"','",E74,"','",F74,"','",G74,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','tent','Blended','tent.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
         <v>7</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D75" t="s">
+        <v>25</v>
+      </c>
+      <c r="E75" t="s">
+        <v>261</v>
+      </c>
+      <c r="F75" t="s">
+        <v>86</v>
+      </c>
+      <c r="G75" t="str">
+        <f>E75&amp;".jpg"</f>
+        <v>cockerel.jpg</v>
+      </c>
+      <c r="H75">
+        <v>4</v>
+      </c>
+      <c r="I75" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D75,"','",E75,"','",F75,"','",G75,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','cockerel','Blended','cockerel.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>29</v>
+      </c>
+      <c r="E76" t="s">
+        <v>262</v>
+      </c>
+      <c r="F76" t="s">
+        <v>86</v>
+      </c>
+      <c r="G76" t="str">
+        <f>E76&amp;".jpg"</f>
+        <v>window.jpg</v>
+      </c>
+      <c r="H76">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I76" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D76,"','",E76,"','",F76,"','",G76,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','window','Blended','window.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" t="s">
+        <v>263</v>
+      </c>
+      <c r="F77" t="s">
+        <v>86</v>
+      </c>
+      <c r="G77" t="str">
+        <f>E77&amp;".jpg"</f>
+        <v>daddy.jpg</v>
+      </c>
+      <c r="H77">
+        <v>4</v>
+      </c>
+      <c r="I77" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D77,"','",E77,"','",F77,"','",G77,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','daddy','Blended','daddy.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" t="s">
+        <v>264</v>
+      </c>
+      <c r="F78" t="s">
+        <v>86</v>
+      </c>
+      <c r="G78" t="str">
+        <f>E78&amp;".jpg"</f>
+        <v>goggles.jpg</v>
+      </c>
+      <c r="H78">
+        <v>4</v>
+      </c>
+      <c r="I78" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D78,"','",E78,"','",F78,"','",G78,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','goggles','Blended','goggles.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>9</v>
+      </c>
+      <c r="D79" t="s">
+        <v>41</v>
+      </c>
+      <c r="E79" t="s">
+        <v>265</v>
+      </c>
+      <c r="F79" t="s">
+        <v>86</v>
+      </c>
+      <c r="G79" t="str">
+        <f>E79&amp;".jpg"</f>
+        <v>fifteen.jpg</v>
+      </c>
+      <c r="H79">
+        <v>4</v>
+      </c>
+      <c r="I79" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D79,"','",E79,"','",F79,"','",G79,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fifteen','Blended','fifteen.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>12</v>
+      </c>
+      <c r="D80" t="s">
+        <v>45</v>
+      </c>
+      <c r="E80" t="s">
+        <v>266</v>
+      </c>
+      <c r="F80" t="s">
+        <v>86</v>
+      </c>
+      <c r="G80" t="str">
+        <f>E80&amp;".jpg"</f>
+        <v>swinging.jpg</v>
+      </c>
+      <c r="H80">
+        <v>4</v>
+      </c>
+      <c r="I80" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D80,"','",E80,"','",F80,"','",G80,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','swinging','Blended','swinging.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>17</v>
+      </c>
+      <c r="D81" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" t="s">
+        <v>267</v>
+      </c>
+      <c r="F81" t="s">
+        <v>86</v>
+      </c>
+      <c r="G81" t="str">
+        <f>E81&amp;".jpg"</f>
+        <v>lollipop.jpg</v>
+      </c>
+      <c r="H81">
+        <v>6</v>
+      </c>
+      <c r="I81" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D81,"','",E81,"','",F81,"','",G81,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','lollipop','Blended','lollipop.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>14</v>
+      </c>
+      <c r="D82" t="s">
+        <v>51</v>
+      </c>
+      <c r="E82" t="s">
+        <v>268</v>
+      </c>
+      <c r="F82" t="s">
+        <v>86</v>
+      </c>
+      <c r="G82" t="str">
+        <f>E82&amp;".jpg"</f>
+        <v>buses.jpg</v>
+      </c>
+      <c r="H82">
+        <v>6</v>
+      </c>
+      <c r="I82" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D82,"','",E82,"','",F82,"','",G82,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','buses','Blended','buses.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>13</v>
+      </c>
+      <c r="D83" t="s">
+        <v>57</v>
+      </c>
+      <c r="E83" t="s">
+        <v>269</v>
+      </c>
+      <c r="F83" t="s">
+        <v>86</v>
+      </c>
+      <c r="G83" t="str">
+        <f>E83&amp;".jpg"</f>
+        <v>yoyo.jpg</v>
+      </c>
+      <c r="H83">
+        <v>4</v>
+      </c>
+      <c r="I83" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D83,"','",E83,"','",F83,"','",G83,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yoyo','Blended','yoyo.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>20</v>
+      </c>
+      <c r="D84" t="s">
+        <v>60</v>
+      </c>
+      <c r="E84" t="s">
+        <v>270</v>
+      </c>
+      <c r="F84" t="s">
+        <v>86</v>
+      </c>
+      <c r="G84" t="str">
+        <f>E84&amp;".jpg"</f>
+        <v>church.jpg</v>
+      </c>
+      <c r="H84">
+        <v>7</v>
+      </c>
+      <c r="I84" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D84,"','",E84,"','",F84,"','",G84,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','church','Blended','church.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85">
         <v>84</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>lemon.jpg</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','lemon','Medial','lemon.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D5" s="19">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>pen.jpg</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','pen','Initial','pen.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="33">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B85">
+        <v>24</v>
+      </c>
+      <c r="D85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" t="s">
+        <v>271</v>
+      </c>
+      <c r="F85" t="s">
+        <v>86</v>
+      </c>
+      <c r="G85" t="str">
+        <f>E85&amp;".jpg"</f>
+        <v>robber.jpg</v>
+      </c>
+      <c r="H85">
+        <v>8</v>
+      </c>
+      <c r="I85" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D85,"','",E85,"','",F85,"','",G85,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','robber','Blended','robber.jpg', 'EN');</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86">
         <v>85</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>map.jpg</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','map','Final','map.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="26">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>teapot.jpg</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','teapot','Medial','teapot.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="19">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>hen.jpg</v>
-      </c>
-      <c r="G8" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hen','Initial','hen.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="19">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>boot.jpg</v>
-      </c>
-      <c r="G9" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','boot','Initial','boot.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="33">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>cub.jpg</v>
-      </c>
-      <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','cub','Final','cub.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B86">
         <v>19</v>
       </c>
-      <c r="D11" s="26">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>robot.jpg</v>
-      </c>
-      <c r="G11" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','robot','Medial','robot.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="19">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>wolf.jpg</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','wolf','Initial','wolf.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="33">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>cow.jpg</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','cow','Final','cow.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="26">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>tower.jpg</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','tower','Medial','tower.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="19">
-        <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>train.jpg</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','train','Initial','train.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>6</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="33">
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>hat.jpg</v>
-      </c>
-      <c r="G16" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','hat','Final','hat.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="26">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>water.jpg</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','water','Medial','water.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
+      <c r="D86" t="s">
+        <v>67</v>
+      </c>
+      <c r="E86" t="s">
+        <v>272</v>
+      </c>
+      <c r="F86" t="s">
+        <v>86</v>
+      </c>
+      <c r="G86" t="str">
+        <f>E86&amp;".jpg"</f>
+        <v>george.jpg</v>
+      </c>
+      <c r="H86">
         <v>7</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="19">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>cat.jpg</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','cat','Initial','cat.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="33">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>sock.jpg</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','sock','Final','sock.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="26">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>rocket.jpg</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','rocket','Medial','rocket.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21">
-        <v>8</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="19">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>gate.jpg</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gate','Initial','gate.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22">
-        <v>8</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="33">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>bag.jpg</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','bag','Final','bag.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23">
-        <v>8</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="26">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>tiger.jpg</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','tiger','Medial','tiger.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24">
-        <v>9</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="D24" s="19">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>fan.jpg</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fan','Initial','fan.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25">
-        <v>9</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="33">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v>laugh.jpg</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','laugh','Final','laugh.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26">
-        <v>9</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="26">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v>wafer.jpg</v>
-      </c>
-      <c r="G26" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','wafer','Medial','wafer.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="19">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v>dog.jpg</v>
-      </c>
-      <c r="G27" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','dog','Initial','dog.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28">
-        <v>10</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="33">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>head.jpg</v>
-      </c>
-      <c r="G28" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','head','Final','head.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29">
-        <v>10</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="26">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v>puddle.jpg</v>
-      </c>
-      <c r="G29" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','puddle','Medial','puddle.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30">
-        <v>11</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="19">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v>nut.jpg</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','nut','Initial','nut.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31">
-        <v>11</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="33">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v>pin.jpg</v>
-      </c>
-      <c r="G31" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','pin','Final','pin.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32">
-        <v>11</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="26">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v>dinner.jpg</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','dinner','Medial','dinner.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33">
-        <v>12</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="33">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" t="str">
-        <f t="shared" si="0"/>
-        <v>wing.jpg</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','wing','Final','wing.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34">
-        <v>12</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="26">
-        <v>3</v>
-      </c>
-      <c r="E34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F34" t="str">
-        <f t="shared" ref="F34:F68" si="2">C34&amp;".jpg"</f>
-        <v>finger.jpg</v>
-      </c>
-      <c r="G34" t="str">
-        <f t="shared" ref="G34:G65" si="3">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",B34,"','",C34,"','",E34,"','",F34,"', 'EN');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','finger','Medial','finger.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35">
-        <v>13</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" s="19">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>83</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="2"/>
-        <v>yak.jpg</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yak','Initial','yak.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36">
-        <v>13</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="D36" s="33">
-        <v>2</v>
-      </c>
-      <c r="E36" t="s">
-        <v>85</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="2"/>
-        <v>boy.jpg</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','boy','Final','boy.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37">
-        <v>13</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" s="26">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="2"/>
-        <v>crayon.jpg</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','crayon','Medial','crayon.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38">
-        <v>14</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="19">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" si="2"/>
-        <v>sun.jpg</v>
-      </c>
-      <c r="G38" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','sun','Initial','sun.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39">
-        <v>14</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D39" s="33">
-        <v>2</v>
-      </c>
-      <c r="E39" t="s">
-        <v>85</v>
-      </c>
-      <c r="F39" t="str">
-        <f t="shared" si="2"/>
-        <v>mouse.jpg</v>
-      </c>
-      <c r="G39" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','mouse','Final','mouse.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40">
-        <v>14</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D40" s="26">
-        <v>3</v>
-      </c>
-      <c r="E40" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" t="str">
-        <f t="shared" si="2"/>
-        <v>listen.jpg</v>
-      </c>
-      <c r="G40" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','listen','Medial','listen.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41">
-        <v>15</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="19">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" si="2"/>
-        <v>shower.jpg</v>
-      </c>
-      <c r="G41" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','shower','Initial','shower.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42">
-        <v>15</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="33">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" t="str">
-        <f t="shared" si="2"/>
-        <v>fish.jpg</v>
-      </c>
-      <c r="G42" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','fish','Final','fish.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43">
-        <v>15</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="D43" s="26">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" t="str">
-        <f t="shared" si="2"/>
-        <v>mushroom.jpg</v>
-      </c>
-      <c r="G43" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','mushroom','Medial','mushroom.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44">
-        <v>16</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="D44" s="19">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>83</v>
-      </c>
-      <c r="F44" t="str">
-        <f t="shared" si="2"/>
-        <v>zip.jpg</v>
-      </c>
-      <c r="G44" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','zip','Initial','zip.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45">
-        <v>16</v>
-      </c>
-      <c r="B45" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="C45" s="30" t="s">
-        <v>242</v>
-      </c>
-      <c r="D45" s="33">
-        <v>2</v>
-      </c>
-      <c r="E45" t="s">
-        <v>85</v>
-      </c>
-      <c r="F45" t="str">
-        <f t="shared" si="2"/>
-        <v>bees.jpg</v>
-      </c>
-      <c r="G45" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','bees','Final','bees.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46">
-        <v>16</v>
-      </c>
-      <c r="B46" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="C46" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="D46" s="26">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>84</v>
-      </c>
-      <c r="F46" t="str">
-        <f t="shared" si="2"/>
-        <v>puzzle.jpg</v>
-      </c>
-      <c r="G46" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','puzzle','Medial','puzzle.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47">
-        <v>17</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" s="19">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>83</v>
-      </c>
-      <c r="F47" t="str">
-        <f t="shared" si="2"/>
-        <v>log.jpg</v>
-      </c>
-      <c r="G47" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','log','Initial','log.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48">
-        <v>17</v>
-      </c>
-      <c r="B48" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="33">
-        <v>2</v>
-      </c>
-      <c r="E48" t="s">
-        <v>85</v>
-      </c>
-      <c r="F48" t="str">
-        <f t="shared" si="2"/>
-        <v>hill.jpg</v>
-      </c>
-      <c r="G48" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','hill','Final','hill.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49">
-        <v>17</v>
-      </c>
-      <c r="B49" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="26">
-        <v>3</v>
-      </c>
-      <c r="E49" t="s">
-        <v>84</v>
-      </c>
-      <c r="F49" t="str">
-        <f t="shared" si="2"/>
-        <v>tulip.jpg</v>
-      </c>
-      <c r="G49" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','tulip','Medial','tulip.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50">
-        <v>18</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="19">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
-        <v>83</v>
-      </c>
-      <c r="F50" t="str">
-        <f t="shared" si="2"/>
-        <v>van.jpg</v>
-      </c>
-      <c r="G50" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','van','Initial','van.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51">
-        <v>18</v>
-      </c>
-      <c r="B51" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" s="33">
-        <v>2</v>
-      </c>
-      <c r="E51" t="s">
-        <v>85</v>
-      </c>
-      <c r="F51" t="str">
-        <f t="shared" si="2"/>
-        <v>sieve.jpg</v>
-      </c>
-      <c r="G51" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','sieve','Final','sieve.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52">
-        <v>18</v>
-      </c>
-      <c r="B52" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52" s="26">
-        <v>3</v>
-      </c>
-      <c r="E52" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" t="str">
-        <f t="shared" si="2"/>
-        <v>waving.jpg</v>
-      </c>
-      <c r="G52" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','waving','Medial','waving.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53">
-        <v>19</v>
-      </c>
-      <c r="B53" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="19">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
-        <v>83</v>
-      </c>
-      <c r="F53" t="str">
-        <f t="shared" si="2"/>
-        <v>jam.jpg</v>
-      </c>
-      <c r="G53" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','jam','Initial','jam.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54">
-        <v>19</v>
-      </c>
-      <c r="B54" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" s="33">
-        <v>2</v>
-      </c>
-      <c r="E54" t="s">
-        <v>85</v>
-      </c>
-      <c r="F54" t="str">
-        <f t="shared" si="2"/>
-        <v>midge.jpg</v>
-      </c>
-      <c r="G54" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','midge','Final','midge.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55">
-        <v>19</v>
-      </c>
-      <c r="B55" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55" s="26">
-        <v>3</v>
-      </c>
-      <c r="E55" t="s">
-        <v>84</v>
-      </c>
-      <c r="F55" t="str">
-        <f t="shared" si="2"/>
-        <v>badger.jpg</v>
-      </c>
-      <c r="G55" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','badger','Medial','badger.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56">
-        <v>20</v>
-      </c>
-      <c r="B56" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="D56" s="19">
-        <v>1</v>
-      </c>
-      <c r="E56" t="s">
-        <v>83</v>
-      </c>
-      <c r="F56" t="str">
-        <f t="shared" si="2"/>
-        <v>chip.jpg</v>
-      </c>
-      <c r="G56" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','chip','Initial','chip.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57">
-        <v>20</v>
-      </c>
-      <c r="B57" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D57" s="33">
-        <v>2</v>
-      </c>
-      <c r="E57" t="s">
-        <v>85</v>
-      </c>
-      <c r="F57" t="str">
-        <f t="shared" si="2"/>
-        <v>witch.jpg</v>
-      </c>
-      <c r="G57" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','witch','Final','witch.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58">
-        <v>20</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D58" s="26">
-        <v>3</v>
-      </c>
-      <c r="E58" t="s">
-        <v>84</v>
-      </c>
-      <c r="F58" t="str">
-        <f t="shared" si="2"/>
-        <v>archer.jpg</v>
-      </c>
-      <c r="G58" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','archer','Medial','archer.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59">
-        <v>21</v>
-      </c>
-      <c r="B59" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="C59" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="D59" s="19">
-        <v>1</v>
-      </c>
-      <c r="E59" t="s">
-        <v>83</v>
-      </c>
-      <c r="F59" t="str">
-        <f t="shared" si="2"/>
-        <v>thorn.jpg</v>
-      </c>
-      <c r="G59" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('tho','thorn','Initial','thorn.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60">
-        <v>21</v>
-      </c>
-      <c r="B60" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="D60" s="33">
-        <v>2</v>
-      </c>
-      <c r="E60" t="s">
-        <v>85</v>
-      </c>
-      <c r="F60" t="str">
-        <f t="shared" si="2"/>
-        <v>path.jpg</v>
-      </c>
-      <c r="G60" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('tho','path','Final','path.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61">
-        <v>21</v>
-      </c>
-      <c r="B61" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="D61" s="26">
-        <v>3</v>
-      </c>
-      <c r="E61" t="s">
-        <v>84</v>
-      </c>
-      <c r="F61" t="str">
-        <f t="shared" si="2"/>
-        <v>birthday.jpg</v>
-      </c>
-      <c r="G61" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('tho','birthday','Medial','birthday.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62">
-        <v>22</v>
-      </c>
-      <c r="B62" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="D62" s="19">
-        <v>1</v>
-      </c>
-      <c r="E62" t="s">
-        <v>83</v>
-      </c>
-      <c r="F62" t="str">
-        <f t="shared" si="2"/>
-        <v>them.jpg</v>
-      </c>
-      <c r="G62" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('thv','them','Initial','them.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63">
-        <v>22</v>
-      </c>
-      <c r="B63" s="28" t="s">
-        <v>250</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="D63" s="33">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s">
-        <v>85</v>
-      </c>
-      <c r="F63" t="str">
-        <f t="shared" si="2"/>
-        <v>bathe.jpg</v>
-      </c>
-      <c r="G63" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('thv','bathe','Final','bathe.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64">
-        <v>22</v>
-      </c>
-      <c r="B64" s="28" t="s">
-        <v>250</v>
-      </c>
-      <c r="C64" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="D64" s="26">
-        <v>3</v>
-      </c>
-      <c r="E64" t="s">
-        <v>84</v>
-      </c>
-      <c r="F64" t="str">
-        <f t="shared" si="2"/>
-        <v>father.jpg</v>
-      </c>
-      <c r="G64" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('thv','father','Medial','father.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65">
-        <v>23</v>
-      </c>
-      <c r="B65" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D65" s="26">
-        <v>3</v>
-      </c>
-      <c r="E65" t="s">
-        <v>84</v>
-      </c>
-      <c r="F65" t="str">
-        <f t="shared" si="2"/>
-        <v>measure.jpg</v>
-      </c>
-      <c r="G65" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('zh','measure','Medial','measure.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66">
-        <v>24</v>
-      </c>
-      <c r="B66" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D66" s="19">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
-        <v>83</v>
-      </c>
-      <c r="F66" t="str">
-        <f t="shared" si="2"/>
-        <v>rat.jpg</v>
-      </c>
-      <c r="G66" t="str">
-        <f t="shared" ref="G66:G97" si="4">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",B66,"','",C66,"','",E66,"','",F66,"', 'EN');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','rat','Initial','rat.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67">
-        <v>24</v>
-      </c>
-      <c r="B67" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="33">
-        <v>2</v>
-      </c>
-      <c r="E67" t="s">
-        <v>85</v>
-      </c>
-      <c r="F67" t="str">
-        <f t="shared" si="2"/>
-        <v>car.jpg</v>
-      </c>
-      <c r="G67" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','car','Final','car.jpg', 'EN');</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68">
-        <v>24</v>
-      </c>
-      <c r="B68" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D68" s="26">
-        <v>3</v>
-      </c>
-      <c r="E68" t="s">
-        <v>84</v>
-      </c>
-      <c r="F68" t="str">
-        <f t="shared" si="2"/>
-        <v>barrel.jpg</v>
-      </c>
-      <c r="G68" t="str">
-        <f t="shared" si="4"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','barrel','Medial','barrel.jpg', 'EN');</v>
+      <c r="I86" t="str">
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D86,"','",E86,"','",F86,"','",G86,"', 'EN');")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','george','Blended','george.jpg', 'EN');</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G68">
-    <sortCondition ref="A2:A68"/>
-    <sortCondition ref="D2:D68"/>
+  <autoFilter ref="A1:I86">
+    <sortState ref="A2:I86">
+      <sortCondition ref="A1:A86"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="B2:I68">
+    <sortCondition ref="B2:B68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added language code filter to all DB Calls Added splash screen Created build scripts Updated Nuget Libraries Added language prefix to all images Added missing translations Added Turkish files Added Turkish data in DB
</commit_message>
<xml_diff>
--- a/Doc/articulation_test_eng_v2.xlsx
+++ b/Doc/articulation_test_eng_v2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\SpeechPath\speechpathology\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SpeechPathology\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215F3FEC-7EBB-4264-94EA-F056173D469B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9080" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENG_DATA" sheetId="1" r:id="rId1"/>
@@ -23,10 +24,15 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">ENG_SQL!$A$1:$E$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ENG_SQL (2)'!$A$1:$I$86</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -521,165 +527,6 @@
     <t>gazoz</t>
   </si>
   <si>
-    <t>bardak.png</t>
-  </si>
-  <si>
-    <t>cep.png</t>
-  </si>
-  <si>
-    <t>çocuk.png</t>
-  </si>
-  <si>
-    <t>diş.png</t>
-  </si>
-  <si>
-    <t>fırça.png</t>
-  </si>
-  <si>
-    <t>gözlük.png</t>
-  </si>
-  <si>
-    <t>kedi.png</t>
-  </si>
-  <si>
-    <t>lamba.png</t>
-  </si>
-  <si>
-    <t>makas.png</t>
-  </si>
-  <si>
-    <t>portakal.png</t>
-  </si>
-  <si>
-    <t>resim.png</t>
-  </si>
-  <si>
-    <t>sabun.png</t>
-  </si>
-  <si>
-    <t>şapka.png</t>
-  </si>
-  <si>
-    <t>tabak.png</t>
-  </si>
-  <si>
-    <t>vişne.png</t>
-  </si>
-  <si>
-    <t>yatak.png</t>
-  </si>
-  <si>
-    <t>zil.png</t>
-  </si>
-  <si>
-    <t>kibrit.png</t>
-  </si>
-  <si>
-    <t>gece.png</t>
-  </si>
-  <si>
-    <t>uçak.png</t>
-  </si>
-  <si>
-    <t>ördek.png</t>
-  </si>
-  <si>
-    <t>sünger.png</t>
-  </si>
-  <si>
-    <t>anahtar.png</t>
-  </si>
-  <si>
-    <t>şeker.png</t>
-  </si>
-  <si>
-    <t>telefon.png</t>
-  </si>
-  <si>
-    <t>limon.png</t>
-  </si>
-  <si>
-    <t>salıncak.png</t>
-  </si>
-  <si>
-    <t>süpürge.png</t>
-  </si>
-  <si>
-    <t>kaşık.png</t>
-  </si>
-  <si>
-    <t>yastık.png</t>
-  </si>
-  <si>
-    <t>tavşan.png</t>
-  </si>
-  <si>
-    <t>siyah.png</t>
-  </si>
-  <si>
-    <t>üzüm.png</t>
-  </si>
-  <si>
-    <t>havuç.png</t>
-  </si>
-  <si>
-    <t>puding.png</t>
-  </si>
-  <si>
-    <t>park.png</t>
-  </si>
-  <si>
-    <t>fil.png</t>
-  </si>
-  <si>
-    <t>kalem.png</t>
-  </si>
-  <si>
-    <t>burun.png</t>
-  </si>
-  <si>
-    <t>kalp.png</t>
-  </si>
-  <si>
-    <t>mantar.png</t>
-  </si>
-  <si>
-    <t>dans.png</t>
-  </si>
-  <si>
-    <t>güneş.png</t>
-  </si>
-  <si>
-    <t>at.png</t>
-  </si>
-  <si>
-    <t>ev.png</t>
-  </si>
-  <si>
-    <t>bebek.png</t>
-  </si>
-  <si>
-    <t>çiçek.png</t>
-  </si>
-  <si>
-    <t>dede.png</t>
-  </si>
-  <si>
-    <t>gaga.png</t>
-  </si>
-  <si>
-    <t>mum.png</t>
-  </si>
-  <si>
-    <t>paspas.png</t>
-  </si>
-  <si>
-    <t>rüzgar.png</t>
-  </si>
-  <si>
-    <t>yay.png</t>
-  </si>
-  <si>
     <t>fotograf.jpg</t>
   </si>
   <si>
@@ -716,18 +563,6 @@
     <t>tablet.jpg</t>
   </si>
   <si>
-    <t>cüce.jpg</t>
-  </si>
-  <si>
-    <t>köfte.jpg</t>
-  </si>
-  <si>
-    <t>çay.jpg</t>
-  </si>
-  <si>
-    <t>şişman.jpg</t>
-  </si>
-  <si>
     <t>gazoz.jpg</t>
   </si>
   <si>
@@ -861,12 +696,183 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>bardak.jpg</t>
+  </si>
+  <si>
+    <t>cep.jpg</t>
+  </si>
+  <si>
+    <t>kedi.jpg</t>
+  </si>
+  <si>
+    <t>lamba.jpg</t>
+  </si>
+  <si>
+    <t>makas.jpg</t>
+  </si>
+  <si>
+    <t>portakal.jpg</t>
+  </si>
+  <si>
+    <t>resim.jpg</t>
+  </si>
+  <si>
+    <t>sabun.jpg</t>
+  </si>
+  <si>
+    <t>tabak.jpg</t>
+  </si>
+  <si>
+    <t>yatak.jpg</t>
+  </si>
+  <si>
+    <t>zil.jpg</t>
+  </si>
+  <si>
+    <t>kibrit.jpg</t>
+  </si>
+  <si>
+    <t>gece.jpg</t>
+  </si>
+  <si>
+    <t>anahtar.jpg</t>
+  </si>
+  <si>
+    <t>telefon.jpg</t>
+  </si>
+  <si>
+    <t>limon.jpg</t>
+  </si>
+  <si>
+    <t>siyah.jpg</t>
+  </si>
+  <si>
+    <t>puding.jpg</t>
+  </si>
+  <si>
+    <t>park.jpg</t>
+  </si>
+  <si>
+    <t>fil.jpg</t>
+  </si>
+  <si>
+    <t>kalem.jpg</t>
+  </si>
+  <si>
+    <t>burun.jpg</t>
+  </si>
+  <si>
+    <t>kalp.jpg</t>
+  </si>
+  <si>
+    <t>mantar.jpg</t>
+  </si>
+  <si>
+    <t>dans.jpg</t>
+  </si>
+  <si>
+    <t>at.jpg</t>
+  </si>
+  <si>
+    <t>ev.jpg</t>
+  </si>
+  <si>
+    <t>bebek.jpg</t>
+  </si>
+  <si>
+    <t>dede.jpg</t>
+  </si>
+  <si>
+    <t>gaga.jpg</t>
+  </si>
+  <si>
+    <t>mum.jpg</t>
+  </si>
+  <si>
+    <t>paspas.jpg</t>
+  </si>
+  <si>
+    <t>yay.jpg</t>
+  </si>
+  <si>
+    <t>cocuk.jpg</t>
+  </si>
+  <si>
+    <t>ucak.jpg</t>
+  </si>
+  <si>
+    <t>havuc.jpg</t>
+  </si>
+  <si>
+    <t>cay.jpg</t>
+  </si>
+  <si>
+    <t>cicek.jpg</t>
+  </si>
+  <si>
+    <t>dis.jpg</t>
+  </si>
+  <si>
+    <t>sapka.jpg</t>
+  </si>
+  <si>
+    <t>visne.jpg</t>
+  </si>
+  <si>
+    <t>seker.jpg</t>
+  </si>
+  <si>
+    <t>tavsan.jpg</t>
+  </si>
+  <si>
+    <t>sisman.jpg</t>
+  </si>
+  <si>
+    <t>ordek.jpg</t>
+  </si>
+  <si>
+    <t>kofte.jpg</t>
+  </si>
+  <si>
+    <t>gozluk.jpg</t>
+  </si>
+  <si>
+    <t>sunger.jpg</t>
+  </si>
+  <si>
+    <t>supurge.jpg</t>
+  </si>
+  <si>
+    <t>uzum.jpg</t>
+  </si>
+  <si>
+    <t>gunes.jpg</t>
+  </si>
+  <si>
+    <t>cuce.jpg</t>
+  </si>
+  <si>
+    <t>ruzgar.jpg</t>
+  </si>
+  <si>
+    <t>firca.jpg</t>
+  </si>
+  <si>
+    <t>salincak.jpg</t>
+  </si>
+  <si>
+    <t>kasik.jpg</t>
+  </si>
+  <si>
+    <t>yastik.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -1098,7 +1104,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1409,23 +1415,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5">
+    <row r="1" spans="1:7" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1448,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="15.5">
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -1453,21 +1459,21 @@
         <v>7</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.5">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>16</v>
@@ -1476,7 +1482,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.5">
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1493,7 +1499,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.5">
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="12" t="s">
         <v>17</v>
       </c>
@@ -1510,7 +1516,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.5">
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="12" t="s">
         <v>29</v>
       </c>
@@ -1527,7 +1533,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.5">
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" s="15" t="s">
         <v>21</v>
       </c>
@@ -1544,7 +1550,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.5">
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="15" t="s">
         <v>25</v>
       </c>
@@ -1561,7 +1567,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="15.5">
+    <row r="9" spans="1:7" ht="15">
       <c r="A9" s="15" t="s">
         <v>37</v>
       </c>
@@ -1578,12 +1584,12 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.5">
+    <row r="10" spans="1:7" ht="15">
       <c r="A10" s="15" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>43</v>
@@ -1595,7 +1601,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.5">
+    <row r="11" spans="1:7" ht="15">
       <c r="A11" s="15" t="s">
         <v>33</v>
       </c>
@@ -1612,7 +1618,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.5">
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" s="15" t="s">
         <v>8</v>
       </c>
@@ -1629,7 +1635,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.5">
+    <row r="13" spans="1:7" ht="15">
       <c r="A13" s="15" t="s">
         <v>45</v>
       </c>
@@ -1646,7 +1652,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.5">
+    <row r="14" spans="1:7" ht="15">
       <c r="A14" s="15" t="s">
         <v>57</v>
       </c>
@@ -1657,13 +1663,13 @@
         <v>59</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="15.5">
+    <row r="15" spans="1:7" ht="15">
       <c r="A15" s="12" t="s">
         <v>51</v>
       </c>
@@ -1671,16 +1677,16 @@
         <v>52</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>237</v>
+        <v>180</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.5">
+    <row r="16" spans="1:7" ht="15">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>73</v>
@@ -1697,24 +1703,24 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="15.5">
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" s="12" t="s">
         <v>157</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>240</v>
+        <v>183</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>241</v>
+        <v>184</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>242</v>
+        <v>185</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="15.5">
+    <row r="18" spans="1:7" ht="15">
       <c r="A18" s="12" t="s">
         <v>47</v>
       </c>
@@ -1731,7 +1737,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="15.5">
+    <row r="19" spans="1:7" ht="15">
       <c r="A19" s="12" t="s">
         <v>53</v>
       </c>
@@ -1748,7 +1754,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="15.5">
+    <row r="20" spans="1:7" ht="15">
       <c r="A20" s="15" t="s">
         <v>67</v>
       </c>
@@ -1765,12 +1771,12 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="15.5">
+    <row r="21" spans="1:7" ht="15">
       <c r="A21" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>243</v>
+        <v>186</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>61</v>
@@ -1782,15 +1788,15 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="15.5">
+    <row r="22" spans="1:7" ht="15">
       <c r="A22" s="15" t="s">
-        <v>250</v>
+        <v>193</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>245</v>
+        <v>188</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>246</v>
+        <v>189</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>75</v>
@@ -1799,18 +1805,18 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="15.5">
+    <row r="23" spans="1:7" ht="15">
       <c r="A23" s="15" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>248</v>
+        <v>191</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
@@ -1851,35 +1857,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H86" sqref="H2:H86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" customWidth="1"/>
-    <col min="3" max="3" width="8.08984375" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="35" customFormat="1" ht="29">
+    <row r="1" spans="1:9" s="35" customFormat="1" ht="28.8">
       <c r="A1" s="39" t="s">
-        <v>275</v>
+        <v>218</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>252</v>
+        <v>195</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>253</v>
+        <v>196</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>79</v>
@@ -1894,7 +1900,7 @@
         <v>82</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>273</v>
+        <v>216</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>81</v>
@@ -1920,14 +1926,14 @@
         <v>83</v>
       </c>
       <c r="G2" t="str">
-        <f>E2&amp;".jpg"</f>
+        <f t="shared" ref="G2:G33" si="0">E2&amp;".jpg"</f>
         <v>mole.jpg</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D2,"','",E2,"','",F2,"','",G2,"', 'EN');")</f>
+        <f t="shared" ref="I2:I33" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D2,"','",E2,"','",F2,"','",G2,"', 'EN');")</f>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mole','Initial','mole.jpg', 'EN');</v>
       </c>
     </row>
@@ -1945,20 +1951,20 @@
         <v>5</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
       <c r="F3" t="s">
         <v>85</v>
       </c>
       <c r="G3" t="str">
-        <f>E3&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>drum.jpg</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D3,"','",E3,"','",F3,"','",G3,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','drum','Final','drum.jpg', 'EN');</v>
       </c>
     </row>
@@ -1982,14 +1988,14 @@
         <v>84</v>
       </c>
       <c r="G4" t="str">
-        <f>E4&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>lemon.jpg</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D4,"','",E4,"','",F4,"','",G4,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','lemon','Medial','lemon.jpg', 'EN');</v>
       </c>
     </row>
@@ -2007,20 +2013,20 @@
         <v>15</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="F5" t="s">
         <v>83</v>
       </c>
       <c r="G5" t="str">
-        <f>E5&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>pen.jpg</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D5,"','",E5,"','",F5,"','",G5,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','pen','Initial','pen.jpg', 'EN');</v>
       </c>
     </row>
@@ -2044,14 +2050,14 @@
         <v>85</v>
       </c>
       <c r="G6" t="str">
-        <f>E6&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>map.jpg</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D6,"','",E6,"','",F6,"','",G6,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','map','Final','map.jpg', 'EN');</v>
       </c>
     </row>
@@ -2069,20 +2075,20 @@
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="F7" t="s">
         <v>84</v>
       </c>
       <c r="G7" t="str">
-        <f>E7&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>teapot.jpg</v>
       </c>
       <c r="H7">
         <v>3</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D7,"','",E7,"','",F7,"','",G7,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','teapot','Medial','teapot.jpg', 'EN');</v>
       </c>
     </row>
@@ -2106,14 +2112,14 @@
         <v>83</v>
       </c>
       <c r="G8" t="str">
-        <f>E8&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>hen.jpg</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D8,"','",E8,"','",F8,"','",G8,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hen','Initial','hen.jpg', 'EN');</v>
       </c>
     </row>
@@ -2137,14 +2143,14 @@
         <v>83</v>
       </c>
       <c r="G9" t="str">
-        <f>E9&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>boot.jpg</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D9,"','",E9,"','",F9,"','",G9,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','boot','Initial','boot.jpg', 'EN');</v>
       </c>
     </row>
@@ -2168,14 +2174,14 @@
         <v>85</v>
       </c>
       <c r="G10" t="str">
-        <f>E10&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>cub.jpg</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D10,"','",E10,"','",F10,"','",G10,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','cub','Final','cub.jpg', 'EN');</v>
       </c>
     </row>
@@ -2199,14 +2205,14 @@
         <v>84</v>
       </c>
       <c r="G11" t="str">
-        <f>E11&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>robot.jpg</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D11,"','",E11,"','",F11,"','",G11,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','robot','Medial','robot.jpg', 'EN');</v>
       </c>
     </row>
@@ -2230,14 +2236,14 @@
         <v>83</v>
       </c>
       <c r="G12" t="str">
-        <f>E12&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>wolf.jpg</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D12,"','",E12,"','",F12,"','",G12,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','wolf','Initial','wolf.jpg', 'EN');</v>
       </c>
     </row>
@@ -2261,14 +2267,14 @@
         <v>85</v>
       </c>
       <c r="G13" t="str">
-        <f>E13&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>cow.jpg</v>
       </c>
       <c r="H13">
         <v>3</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D13,"','",E13,"','",F13,"','",G13,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','cow','Final','cow.jpg', 'EN');</v>
       </c>
     </row>
@@ -2292,14 +2298,14 @@
         <v>84</v>
       </c>
       <c r="G14" t="str">
-        <f>E14&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>tower.jpg</v>
       </c>
       <c r="H14">
         <v>3</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D14,"','",E14,"','",F14,"','",G14,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','tower','Medial','tower.jpg', 'EN');</v>
       </c>
     </row>
@@ -2323,14 +2329,14 @@
         <v>83</v>
       </c>
       <c r="G15" t="str">
-        <f>E15&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>train.jpg</v>
       </c>
       <c r="H15">
         <v>4</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D15,"','",E15,"','",F15,"','",G15,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','train','Initial','train.jpg', 'EN');</v>
       </c>
     </row>
@@ -2354,14 +2360,14 @@
         <v>85</v>
       </c>
       <c r="G16" t="str">
-        <f>E16&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>hat.jpg</v>
       </c>
       <c r="H16">
         <v>4</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D16,"','",E16,"','",F16,"','",G16,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','hat','Final','hat.jpg', 'EN');</v>
       </c>
     </row>
@@ -2385,14 +2391,14 @@
         <v>84</v>
       </c>
       <c r="G17" t="str">
-        <f>E17&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>water.jpg</v>
       </c>
       <c r="H17">
         <v>4</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D17,"','",E17,"','",F17,"','",G17,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','water','Medial','water.jpg', 'EN');</v>
       </c>
     </row>
@@ -2416,14 +2422,14 @@
         <v>83</v>
       </c>
       <c r="G18" t="str">
-        <f>E18&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>cat.jpg</v>
       </c>
       <c r="H18">
         <v>4</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D18,"','",E18,"','",F18,"','",G18,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','cat','Initial','cat.jpg', 'EN');</v>
       </c>
     </row>
@@ -2447,14 +2453,14 @@
         <v>85</v>
       </c>
       <c r="G19" t="str">
-        <f>E19&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>sock.jpg</v>
       </c>
       <c r="H19">
         <v>4</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D19,"','",E19,"','",F19,"','",G19,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','sock','Final','sock.jpg', 'EN');</v>
       </c>
     </row>
@@ -2478,14 +2484,14 @@
         <v>84</v>
       </c>
       <c r="G20" t="str">
-        <f>E20&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>rocket.jpg</v>
       </c>
       <c r="H20">
         <v>4</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D20,"','",E20,"','",F20,"','",G20,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','rocket','Medial','rocket.jpg', 'EN');</v>
       </c>
     </row>
@@ -2509,14 +2515,14 @@
         <v>83</v>
       </c>
       <c r="G21" t="str">
-        <f>E21&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>gate.jpg</v>
       </c>
       <c r="H21">
         <v>4</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D21,"','",E21,"','",F21,"','",G21,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gate','Initial','gate.jpg', 'EN');</v>
       </c>
     </row>
@@ -2540,14 +2546,14 @@
         <v>85</v>
       </c>
       <c r="G22" t="str">
-        <f>E22&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>bag.jpg</v>
       </c>
       <c r="H22">
         <v>4</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D22,"','",E22,"','",F22,"','",G22,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','bag','Final','bag.jpg', 'EN');</v>
       </c>
     </row>
@@ -2571,14 +2577,14 @@
         <v>84</v>
       </c>
       <c r="G23" t="str">
-        <f>E23&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>tiger.jpg</v>
       </c>
       <c r="H23">
         <v>4</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D23,"','",E23,"','",F23,"','",G23,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','tiger','Medial','tiger.jpg', 'EN');</v>
       </c>
     </row>
@@ -2596,20 +2602,20 @@
         <v>41</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="F24" t="s">
         <v>83</v>
       </c>
       <c r="G24" t="str">
-        <f>E24&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>fan.jpg</v>
       </c>
       <c r="H24">
         <v>4</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D24,"','",E24,"','",F24,"','",G24,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fan','Initial','fan.jpg', 'EN');</v>
       </c>
     </row>
@@ -2633,14 +2639,14 @@
         <v>85</v>
       </c>
       <c r="G25" t="str">
-        <f>E25&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>laugh.jpg</v>
       </c>
       <c r="H25">
         <v>4</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D25,"','",E25,"','",F25,"','",G25,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','laugh','Final','laugh.jpg', 'EN');</v>
       </c>
     </row>
@@ -2664,14 +2670,14 @@
         <v>84</v>
       </c>
       <c r="G26" t="str">
-        <f>E26&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>wafer.jpg</v>
       </c>
       <c r="H26">
         <v>4</v>
       </c>
       <c r="I26" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D26,"','",E26,"','",F26,"','",G26,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','wafer','Medial','wafer.jpg', 'EN');</v>
       </c>
     </row>
@@ -2695,14 +2701,14 @@
         <v>83</v>
       </c>
       <c r="G27" t="str">
-        <f>E27&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>dog.jpg</v>
       </c>
       <c r="H27">
         <v>4</v>
       </c>
       <c r="I27" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D27,"','",E27,"','",F27,"','",G27,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','dog','Initial','dog.jpg', 'EN');</v>
       </c>
     </row>
@@ -2726,14 +2732,14 @@
         <v>85</v>
       </c>
       <c r="G28" t="str">
-        <f>E28&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>head.jpg</v>
       </c>
       <c r="H28">
         <v>4</v>
       </c>
       <c r="I28" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D28,"','",E28,"','",F28,"','",G28,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','head','Final','head.jpg', 'EN');</v>
       </c>
     </row>
@@ -2757,14 +2763,14 @@
         <v>84</v>
       </c>
       <c r="G29" t="str">
-        <f>E29&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>puddle.jpg</v>
       </c>
       <c r="H29">
         <v>4</v>
       </c>
       <c r="I29" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D29,"','",E29,"','",F29,"','",G29,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','puddle','Medial','puddle.jpg', 'EN');</v>
       </c>
     </row>
@@ -2788,14 +2794,14 @@
         <v>83</v>
       </c>
       <c r="G30" t="str">
-        <f>E30&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>nut.jpg</v>
       </c>
       <c r="H30">
         <v>4</v>
       </c>
       <c r="I30" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D30,"','",E30,"','",F30,"','",G30,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','nut','Initial','nut.jpg', 'EN');</v>
       </c>
     </row>
@@ -2819,14 +2825,14 @@
         <v>85</v>
       </c>
       <c r="G31" t="str">
-        <f>E31&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>pin.jpg</v>
       </c>
       <c r="H31">
         <v>4</v>
       </c>
       <c r="I31" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D31,"','",E31,"','",F31,"','",G31,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','pin','Final','pin.jpg', 'EN');</v>
       </c>
     </row>
@@ -2850,14 +2856,14 @@
         <v>84</v>
       </c>
       <c r="G32" t="str">
-        <f>E32&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>dinner.jpg</v>
       </c>
       <c r="H32">
         <v>4</v>
       </c>
       <c r="I32" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D32,"','",E32,"','",F32,"','",G32,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','dinner','Medial','dinner.jpg', 'EN');</v>
       </c>
     </row>
@@ -2881,14 +2887,14 @@
         <v>85</v>
       </c>
       <c r="G33" t="str">
-        <f>E33&amp;".jpg"</f>
+        <f t="shared" si="0"/>
         <v>wing.jpg</v>
       </c>
       <c r="H33">
         <v>4</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D33,"','",E33,"','",F33,"','",G33,"', 'EN');")</f>
+        <f t="shared" si="1"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','wing','Final','wing.jpg', 'EN');</v>
       </c>
     </row>
@@ -2912,14 +2918,14 @@
         <v>84</v>
       </c>
       <c r="G34" t="str">
-        <f>E34&amp;".jpg"</f>
+        <f t="shared" ref="G34:G65" si="2">E34&amp;".jpg"</f>
         <v>finger.jpg</v>
       </c>
       <c r="H34">
         <v>4</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D34,"','",E34,"','",F34,"','",G34,"', 'EN');")</f>
+        <f t="shared" ref="I34:I65" si="3">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D34,"','",E34,"','",F34,"','",G34,"', 'EN');")</f>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','finger','Medial','finger.jpg', 'EN');</v>
       </c>
     </row>
@@ -2943,14 +2949,14 @@
         <v>83</v>
       </c>
       <c r="G35" t="str">
-        <f>E35&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>yak.jpg</v>
       </c>
       <c r="H35">
         <v>4</v>
       </c>
       <c r="I35" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D35,"','",E35,"','",F35,"','",G35,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yak','Initial','yak.jpg', 'EN');</v>
       </c>
     </row>
@@ -2968,20 +2974,20 @@
         <v>57</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
       <c r="F36" t="s">
         <v>85</v>
       </c>
       <c r="G36" t="str">
-        <f>E36&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>boy.jpg</v>
       </c>
       <c r="H36">
         <v>4</v>
       </c>
       <c r="I36" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D36,"','",E36,"','",F36,"','",G36,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','boy','Final','boy.jpg', 'EN');</v>
       </c>
     </row>
@@ -3005,14 +3011,14 @@
         <v>84</v>
       </c>
       <c r="G37" t="str">
-        <f>E37&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>crayon.jpg</v>
       </c>
       <c r="H37">
         <v>4</v>
       </c>
       <c r="I37" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D37,"','",E37,"','",F37,"','",G37,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','crayon','Medial','crayon.jpg', 'EN');</v>
       </c>
     </row>
@@ -3036,14 +3042,14 @@
         <v>83</v>
       </c>
       <c r="G38" t="str">
-        <f>E38&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>sun.jpg</v>
       </c>
       <c r="H38">
         <v>6</v>
       </c>
       <c r="I38" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D38,"','",E38,"','",F38,"','",G38,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','sun','Initial','sun.jpg', 'EN');</v>
       </c>
     </row>
@@ -3061,20 +3067,20 @@
         <v>51</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="F39" t="s">
         <v>85</v>
       </c>
       <c r="G39" t="str">
-        <f>E39&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>mouse.jpg</v>
       </c>
       <c r="H39">
         <v>6</v>
       </c>
       <c r="I39" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D39,"','",E39,"','",F39,"','",G39,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','mouse','Final','mouse.jpg', 'EN');</v>
       </c>
     </row>
@@ -3092,20 +3098,20 @@
         <v>51</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>237</v>
+        <v>180</v>
       </c>
       <c r="F40" t="s">
         <v>84</v>
       </c>
       <c r="G40" t="str">
-        <f>E40&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>listen.jpg</v>
       </c>
       <c r="H40">
         <v>6</v>
       </c>
       <c r="I40" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D40,"','",E40,"','",F40,"','",G40,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','listen','Medial','listen.jpg', 'EN');</v>
       </c>
     </row>
@@ -3129,14 +3135,14 @@
         <v>83</v>
       </c>
       <c r="G41" t="str">
-        <f>E41&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>shower.jpg</v>
       </c>
       <c r="H41">
         <v>6</v>
       </c>
       <c r="I41" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D41,"','",E41,"','",F41,"','",G41,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','shower','Initial','shower.jpg', 'EN');</v>
       </c>
     </row>
@@ -3160,14 +3166,14 @@
         <v>85</v>
       </c>
       <c r="G42" t="str">
-        <f>E42&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>fish.jpg</v>
       </c>
       <c r="H42">
         <v>6</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D42,"','",E42,"','",F42,"','",G42,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','fish','Final','fish.jpg', 'EN');</v>
       </c>
     </row>
@@ -3185,20 +3191,20 @@
         <v>71</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
       <c r="F43" t="s">
         <v>84</v>
       </c>
       <c r="G43" t="str">
-        <f>E43&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>mushroom.jpg</v>
       </c>
       <c r="H43">
         <v>6</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D43,"','",E43,"','",F43,"','",G43,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('sh','mushroom','Medial','mushroom.jpg', 'EN');</v>
       </c>
     </row>
@@ -3216,20 +3222,20 @@
         <v>157</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>240</v>
+        <v>183</v>
       </c>
       <c r="F44" t="s">
         <v>83</v>
       </c>
       <c r="G44" t="str">
-        <f>E44&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>zip.jpg</v>
       </c>
       <c r="H44">
         <v>6</v>
       </c>
       <c r="I44" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D44,"','",E44,"','",F44,"','",G44,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','zip','Initial','zip.jpg', 'EN');</v>
       </c>
     </row>
@@ -3247,20 +3253,20 @@
         <v>157</v>
       </c>
       <c r="E45" s="30" t="s">
-        <v>242</v>
+        <v>185</v>
       </c>
       <c r="F45" t="s">
         <v>85</v>
       </c>
       <c r="G45" t="str">
-        <f>E45&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>bees.jpg</v>
       </c>
       <c r="H45">
         <v>6</v>
       </c>
       <c r="I45" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D45,"','",E45,"','",F45,"','",G45,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','bees','Final','bees.jpg', 'EN');</v>
       </c>
     </row>
@@ -3278,20 +3284,20 @@
         <v>157</v>
       </c>
       <c r="E46" s="30" t="s">
-        <v>241</v>
+        <v>184</v>
       </c>
       <c r="F46" t="s">
         <v>84</v>
       </c>
       <c r="G46" t="str">
-        <f>E46&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>puzzle.jpg</v>
       </c>
       <c r="H46">
         <v>6</v>
       </c>
       <c r="I46" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D46,"','",E46,"','",F46,"','",G46,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','puzzle','Medial','puzzle.jpg', 'EN');</v>
       </c>
     </row>
@@ -3315,14 +3321,14 @@
         <v>83</v>
       </c>
       <c r="G47" t="str">
-        <f>E47&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>log.jpg</v>
       </c>
       <c r="H47">
         <v>6</v>
       </c>
       <c r="I47" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D47,"','",E47,"','",F47,"','",G47,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','log','Initial','log.jpg', 'EN');</v>
       </c>
     </row>
@@ -3346,14 +3352,14 @@
         <v>85</v>
       </c>
       <c r="G48" t="str">
-        <f>E48&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>hill.jpg</v>
       </c>
       <c r="H48">
         <v>6</v>
       </c>
       <c r="I48" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D48,"','",E48,"','",F48,"','",G48,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','hill','Final','hill.jpg', 'EN');</v>
       </c>
     </row>
@@ -3377,14 +3383,14 @@
         <v>84</v>
       </c>
       <c r="G49" t="str">
-        <f>E49&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>tulip.jpg</v>
       </c>
       <c r="H49">
         <v>6</v>
       </c>
       <c r="I49" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D49,"','",E49,"','",F49,"','",G49,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','tulip','Medial','tulip.jpg', 'EN');</v>
       </c>
     </row>
@@ -3408,14 +3414,14 @@
         <v>83</v>
       </c>
       <c r="G50" t="str">
-        <f>E50&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>van.jpg</v>
       </c>
       <c r="H50">
         <v>6</v>
       </c>
       <c r="I50" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D50,"','",E50,"','",F50,"','",G50,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','van','Initial','van.jpg', 'EN');</v>
       </c>
     </row>
@@ -3439,14 +3445,14 @@
         <v>85</v>
       </c>
       <c r="G51" t="str">
-        <f>E51&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>sieve.jpg</v>
       </c>
       <c r="H51">
         <v>6</v>
       </c>
       <c r="I51" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D51,"','",E51,"','",F51,"','",G51,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','sieve','Final','sieve.jpg', 'EN');</v>
       </c>
     </row>
@@ -3470,14 +3476,14 @@
         <v>84</v>
       </c>
       <c r="G52" t="str">
-        <f>E52&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>waving.jpg</v>
       </c>
       <c r="H52">
         <v>6</v>
       </c>
       <c r="I52" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D52,"','",E52,"','",F52,"','",G52,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','waving','Medial','waving.jpg', 'EN');</v>
       </c>
     </row>
@@ -3501,14 +3507,14 @@
         <v>83</v>
       </c>
       <c r="G53" t="str">
-        <f>E53&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>jam.jpg</v>
       </c>
       <c r="H53">
         <v>7</v>
       </c>
       <c r="I53" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D53,"','",E53,"','",F53,"','",G53,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','jam','Initial','jam.jpg', 'EN');</v>
       </c>
     </row>
@@ -3532,14 +3538,14 @@
         <v>85</v>
       </c>
       <c r="G54" t="str">
-        <f>E54&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>midge.jpg</v>
       </c>
       <c r="H54">
         <v>7</v>
       </c>
       <c r="I54" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D54,"','",E54,"','",F54,"','",G54,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','midge','Final','midge.jpg', 'EN');</v>
       </c>
     </row>
@@ -3563,14 +3569,14 @@
         <v>84</v>
       </c>
       <c r="G55" t="str">
-        <f>E55&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>badger.jpg</v>
       </c>
       <c r="H55">
         <v>7</v>
       </c>
       <c r="I55" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D55,"','",E55,"','",F55,"','",G55,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','badger','Medial','badger.jpg', 'EN');</v>
       </c>
     </row>
@@ -3588,20 +3594,20 @@
         <v>60</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="F56" t="s">
         <v>83</v>
       </c>
       <c r="G56" t="str">
-        <f>E56&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>chips.jpg</v>
       </c>
       <c r="H56">
         <v>7</v>
       </c>
       <c r="I56" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D56,"','",E56,"','",F56,"','",G56,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','chips','Initial','chips.jpg', 'EN');</v>
       </c>
     </row>
@@ -3625,14 +3631,14 @@
         <v>85</v>
       </c>
       <c r="G57" t="str">
-        <f>E57&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>witch.jpg</v>
       </c>
       <c r="H57">
         <v>7</v>
       </c>
       <c r="I57" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D57,"','",E57,"','",F57,"','",G57,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','witch','Final','witch.jpg', 'EN');</v>
       </c>
     </row>
@@ -3656,14 +3662,14 @@
         <v>84</v>
       </c>
       <c r="G58" t="str">
-        <f>E58&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>archer.jpg</v>
       </c>
       <c r="H58">
         <v>7</v>
       </c>
       <c r="I58" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D58,"','",E58,"','",F58,"','",G58,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','archer','Medial','archer.jpg', 'EN');</v>
       </c>
     </row>
@@ -3678,23 +3684,23 @@
         <v>1</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>245</v>
+        <v>188</v>
       </c>
       <c r="F59" t="s">
         <v>83</v>
       </c>
       <c r="G59" t="str">
-        <f>E59&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>thorn.jpg</v>
       </c>
       <c r="H59">
         <v>7</v>
       </c>
       <c r="I59" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D59,"','",E59,"','",F59,"','",G59,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','thorn','Initial','thorn.jpg', 'EN');</v>
       </c>
     </row>
@@ -3709,7 +3715,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="E60" s="29" t="s">
         <v>75</v>
@@ -3718,14 +3724,14 @@
         <v>85</v>
       </c>
       <c r="G60" t="str">
-        <f>E60&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>path.jpg</v>
       </c>
       <c r="H60">
         <v>7</v>
       </c>
       <c r="I60" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D60,"','",E60,"','",F60,"','",G60,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','path','Final','path.jpg', 'EN');</v>
       </c>
     </row>
@@ -3740,23 +3746,23 @@
         <v>3</v>
       </c>
       <c r="D61" s="28" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>246</v>
+        <v>189</v>
       </c>
       <c r="F61" t="s">
         <v>84</v>
       </c>
       <c r="G61" t="str">
-        <f>E61&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>birthday.jpg</v>
       </c>
       <c r="H61">
         <v>7</v>
       </c>
       <c r="I61" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D61,"','",E61,"','",F61,"','",G61,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','birthday','Medial','birthday.jpg', 'EN');</v>
       </c>
     </row>
@@ -3771,23 +3777,23 @@
         <v>1</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>248</v>
+        <v>191</v>
       </c>
       <c r="F62" t="s">
         <v>83</v>
       </c>
       <c r="G62" t="str">
-        <f>E62&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>them.jpg</v>
       </c>
       <c r="H62">
         <v>7</v>
       </c>
       <c r="I62" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D62,"','",E62,"','",F62,"','",G62,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','them','Initial','them.jpg', 'EN');</v>
       </c>
     </row>
@@ -3802,23 +3808,23 @@
         <v>2</v>
       </c>
       <c r="D63" s="28" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="F63" t="s">
         <v>85</v>
       </c>
       <c r="G63" t="str">
-        <f>E63&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>bathe.jpg</v>
       </c>
       <c r="H63">
         <v>7</v>
       </c>
       <c r="I63" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D63,"','",E63,"','",F63,"','",G63,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','bathe','Final','bathe.jpg', 'EN');</v>
       </c>
     </row>
@@ -3833,7 +3839,7 @@
         <v>3</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="E64" s="29" t="s">
         <v>74</v>
@@ -3842,14 +3848,14 @@
         <v>84</v>
       </c>
       <c r="G64" t="str">
-        <f>E64&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>father.jpg</v>
       </c>
       <c r="H64">
         <v>7</v>
       </c>
       <c r="I64" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D64,"','",E64,"','",F64,"','",G64,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('th','father','Medial','father.jpg', 'EN');</v>
       </c>
     </row>
@@ -3873,14 +3879,14 @@
         <v>84</v>
       </c>
       <c r="G65" t="str">
-        <f>E65&amp;".jpg"</f>
+        <f t="shared" si="2"/>
         <v>measure.jpg</v>
       </c>
       <c r="H65">
         <v>8</v>
       </c>
       <c r="I65" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D65,"','",E65,"','",F65,"','",G65,"', 'EN');")</f>
+        <f t="shared" si="3"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('zh','measure','Medial','measure.jpg', 'EN');</v>
       </c>
     </row>
@@ -3904,14 +3910,14 @@
         <v>83</v>
       </c>
       <c r="G66" t="str">
-        <f>E66&amp;".jpg"</f>
+        <f t="shared" ref="G66:G86" si="4">E66&amp;".jpg"</f>
         <v>rat.jpg</v>
       </c>
       <c r="H66">
         <v>8</v>
       </c>
       <c r="I66" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D66,"','",E66,"','",F66,"','",G66,"', 'EN');")</f>
+        <f t="shared" ref="I66:I86" si="5">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D66,"','",E66,"','",F66,"','",G66,"', 'EN');")</f>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','rat','Initial','rat.jpg', 'EN');</v>
       </c>
     </row>
@@ -3935,14 +3941,14 @@
         <v>85</v>
       </c>
       <c r="G67" t="str">
-        <f>E67&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>car.jpg</v>
       </c>
       <c r="H67">
         <v>8</v>
       </c>
       <c r="I67" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D67,"','",E67,"','",F67,"','",G67,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','car','Final','car.jpg', 'EN');</v>
       </c>
     </row>
@@ -3966,14 +3972,14 @@
         <v>84</v>
       </c>
       <c r="G68" t="str">
-        <f>E68&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>barrel.jpg</v>
       </c>
       <c r="H68">
         <v>8</v>
       </c>
       <c r="I68" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D68,"','",E68,"','",F68,"','",G68,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','barrel','Medial','barrel.jpg', 'EN');</v>
       </c>
     </row>
@@ -3988,20 +3994,20 @@
         <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>255</v>
+        <v>198</v>
       </c>
       <c r="F69" t="s">
         <v>86</v>
       </c>
       <c r="G69" t="str">
-        <f>E69&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>mummy.jpg</v>
       </c>
       <c r="H69">
         <v>3</v>
       </c>
       <c r="I69" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D69,"','",E69,"','",F69,"','",G69,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mummy','Blended','mummy.jpg', 'EN');</v>
       </c>
     </row>
@@ -4016,20 +4022,20 @@
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>256</v>
+        <v>199</v>
       </c>
       <c r="F70" t="s">
         <v>86</v>
       </c>
       <c r="G70" t="str">
-        <f>E70&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>cannon.jpg</v>
       </c>
       <c r="H70">
         <v>4</v>
       </c>
       <c r="I70" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D70,"','",E70,"','",F70,"','",G70,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','cannon','Blended','cannon.jpg', 'EN');</v>
       </c>
     </row>
@@ -4041,20 +4047,20 @@
         <v>12</v>
       </c>
       <c r="E71" t="s">
-        <v>257</v>
+        <v>200</v>
       </c>
       <c r="F71" t="s">
         <v>86</v>
       </c>
       <c r="G71" t="str">
-        <f>E71&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>hardhat.jpg</v>
       </c>
       <c r="H71">
         <v>3</v>
       </c>
       <c r="I71" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D71,"','",E71,"','",F71,"','",G71,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hardhat','Blended','hardhat.jpg', 'EN');</v>
       </c>
     </row>
@@ -4069,20 +4075,20 @@
         <v>15</v>
       </c>
       <c r="E72" t="s">
-        <v>258</v>
+        <v>201</v>
       </c>
       <c r="F72" t="s">
         <v>86</v>
       </c>
       <c r="G72" t="str">
-        <f>E72&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>pepper.jpg</v>
       </c>
       <c r="H72">
         <v>3</v>
       </c>
       <c r="I72" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D72,"','",E72,"','",F72,"','",G72,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','pepper','Blended','pepper.jpg', 'EN');</v>
       </c>
     </row>
@@ -4097,20 +4103,20 @@
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>259</v>
+        <v>202</v>
       </c>
       <c r="F73" t="s">
         <v>86</v>
       </c>
       <c r="G73" t="str">
-        <f>E73&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>baby.jpg</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D73,"','",E73,"','",F73,"','",G73,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','baby','Blended','baby.jpg', 'EN');</v>
       </c>
     </row>
@@ -4125,20 +4131,20 @@
         <v>21</v>
       </c>
       <c r="E74" t="s">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="F74" t="s">
         <v>86</v>
       </c>
       <c r="G74" t="str">
-        <f>E74&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>tent.jpg</v>
       </c>
       <c r="H74">
         <v>4</v>
       </c>
       <c r="I74" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D74,"','",E74,"','",F74,"','",G74,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','tent','Blended','tent.jpg', 'EN');</v>
       </c>
     </row>
@@ -4153,20 +4159,20 @@
         <v>25</v>
       </c>
       <c r="E75" t="s">
-        <v>261</v>
+        <v>204</v>
       </c>
       <c r="F75" t="s">
         <v>86</v>
       </c>
       <c r="G75" t="str">
-        <f>E75&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>cockerel.jpg</v>
       </c>
       <c r="H75">
         <v>4</v>
       </c>
       <c r="I75" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D75,"','",E75,"','",F75,"','",G75,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','cockerel','Blended','cockerel.jpg', 'EN');</v>
       </c>
     </row>
@@ -4181,20 +4187,20 @@
         <v>29</v>
       </c>
       <c r="E76" t="s">
-        <v>262</v>
+        <v>205</v>
       </c>
       <c r="F76" t="s">
         <v>86</v>
       </c>
       <c r="G76" t="str">
-        <f>E76&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>window.jpg</v>
       </c>
       <c r="H76">
         <v>3</v>
       </c>
       <c r="I76" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D76,"','",E76,"','",F76,"','",G76,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('w','window','Blended','window.jpg', 'EN');</v>
       </c>
     </row>
@@ -4209,20 +4215,20 @@
         <v>33</v>
       </c>
       <c r="E77" t="s">
-        <v>263</v>
+        <v>206</v>
       </c>
       <c r="F77" t="s">
         <v>86</v>
       </c>
       <c r="G77" t="str">
-        <f>E77&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>daddy.jpg</v>
       </c>
       <c r="H77">
         <v>4</v>
       </c>
       <c r="I77" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D77,"','",E77,"','",F77,"','",G77,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','daddy','Blended','daddy.jpg', 'EN');</v>
       </c>
     </row>
@@ -4237,20 +4243,20 @@
         <v>37</v>
       </c>
       <c r="E78" t="s">
-        <v>264</v>
+        <v>207</v>
       </c>
       <c r="F78" t="s">
         <v>86</v>
       </c>
       <c r="G78" t="str">
-        <f>E78&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>goggles.jpg</v>
       </c>
       <c r="H78">
         <v>4</v>
       </c>
       <c r="I78" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D78,"','",E78,"','",F78,"','",G78,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','goggles','Blended','goggles.jpg', 'EN');</v>
       </c>
     </row>
@@ -4265,20 +4271,20 @@
         <v>41</v>
       </c>
       <c r="E79" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="F79" t="s">
         <v>86</v>
       </c>
       <c r="G79" t="str">
-        <f>E79&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>fifteen.jpg</v>
       </c>
       <c r="H79">
         <v>4</v>
       </c>
       <c r="I79" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D79,"','",E79,"','",F79,"','",G79,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fifteen','Blended','fifteen.jpg', 'EN');</v>
       </c>
     </row>
@@ -4293,20 +4299,20 @@
         <v>45</v>
       </c>
       <c r="E80" t="s">
-        <v>266</v>
+        <v>209</v>
       </c>
       <c r="F80" t="s">
         <v>86</v>
       </c>
       <c r="G80" t="str">
-        <f>E80&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>swinging.jpg</v>
       </c>
       <c r="H80">
         <v>4</v>
       </c>
       <c r="I80" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D80,"','",E80,"','",F80,"','",G80,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ng','swinging','Blended','swinging.jpg', 'EN');</v>
       </c>
     </row>
@@ -4321,20 +4327,20 @@
         <v>47</v>
       </c>
       <c r="E81" t="s">
-        <v>267</v>
+        <v>210</v>
       </c>
       <c r="F81" t="s">
         <v>86</v>
       </c>
       <c r="G81" t="str">
-        <f>E81&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>lollipop.jpg</v>
       </c>
       <c r="H81">
         <v>6</v>
       </c>
       <c r="I81" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D81,"','",E81,"','",F81,"','",G81,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','lollipop','Blended','lollipop.jpg', 'EN');</v>
       </c>
     </row>
@@ -4349,20 +4355,20 @@
         <v>51</v>
       </c>
       <c r="E82" t="s">
-        <v>268</v>
+        <v>211</v>
       </c>
       <c r="F82" t="s">
         <v>86</v>
       </c>
       <c r="G82" t="str">
-        <f>E82&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>buses.jpg</v>
       </c>
       <c r="H82">
         <v>6</v>
       </c>
       <c r="I82" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D82,"','",E82,"','",F82,"','",G82,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','buses','Blended','buses.jpg', 'EN');</v>
       </c>
     </row>
@@ -4377,20 +4383,20 @@
         <v>57</v>
       </c>
       <c r="E83" t="s">
-        <v>269</v>
+        <v>212</v>
       </c>
       <c r="F83" t="s">
         <v>86</v>
       </c>
       <c r="G83" t="str">
-        <f>E83&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>yoyo.jpg</v>
       </c>
       <c r="H83">
         <v>4</v>
       </c>
       <c r="I83" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D83,"','",E83,"','",F83,"','",G83,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yoyo','Blended','yoyo.jpg', 'EN');</v>
       </c>
     </row>
@@ -4405,20 +4411,20 @@
         <v>60</v>
       </c>
       <c r="E84" t="s">
-        <v>270</v>
+        <v>213</v>
       </c>
       <c r="F84" t="s">
         <v>86</v>
       </c>
       <c r="G84" t="str">
-        <f>E84&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>church.jpg</v>
       </c>
       <c r="H84">
         <v>7</v>
       </c>
       <c r="I84" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D84,"','",E84,"','",F84,"','",G84,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ch','church','Blended','church.jpg', 'EN');</v>
       </c>
     </row>
@@ -4433,20 +4439,20 @@
         <v>63</v>
       </c>
       <c r="E85" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
       <c r="F85" t="s">
         <v>86</v>
       </c>
       <c r="G85" t="str">
-        <f>E85&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>robber.jpg</v>
       </c>
       <c r="H85">
         <v>8</v>
       </c>
       <c r="I85" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D85,"','",E85,"','",F85,"','",G85,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','robber','Blended','robber.jpg', 'EN');</v>
       </c>
     </row>
@@ -4461,25 +4467,25 @@
         <v>67</v>
       </c>
       <c r="E86" t="s">
-        <v>272</v>
+        <v>215</v>
       </c>
       <c r="F86" t="s">
         <v>86</v>
       </c>
       <c r="G86" t="str">
-        <f>E86&amp;".jpg"</f>
+        <f t="shared" si="4"/>
         <v>george.jpg</v>
       </c>
       <c r="H86">
         <v>7</v>
       </c>
       <c r="I86" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",D86,"','",E86,"','",F86,"','",G86,"', 'EN');")</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('j','george','Blended','george.jpg', 'EN');</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I86">
+  <autoFilter ref="A1:I86" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState ref="A2:I86">
       <sortCondition ref="A1:A86"/>
     </sortState>
@@ -4493,14 +4499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
   </cols>
@@ -4843,17 +4849,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D36" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="13.7265625" customWidth="1"/>
-    <col min="5" max="5" width="98.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="98.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4884,11 +4890,11 @@
         <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>219</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A2,"','",B2,"','",C2,"','",D2,"', 'TR');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','bardak','Initial','bardak.png', 'TR');</v>
+        <f>CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('",A2,"','",B2,"','",C2,"','tr_",D2,"', 'TR',0);")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('b','bardak','Initial','tr_bardak.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4902,11 +4908,11 @@
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>220</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A3,"','",B3,"','",C3,"','",D3,"', 'TR');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('c','cep','Initial','cep.png', 'TR');</v>
+        <f t="shared" ref="E3:E66" si="0">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('",A3,"','",B3,"','",C3,"','tr_",D3,"', 'TR',0);")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('c','cep','Initial','tr_cep.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4920,11 +4926,11 @@
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>252</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','çocuk','Initial','çocuk.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ç','çocuk','Initial','tr_cocuk.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4938,11 +4944,11 @@
         <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>257</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','diş','Initial','diş.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('d','diş','Initial','tr_dis.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4956,11 +4962,11 @@
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>272</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fırça','Initial','fırça.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('f','fırça','Initial','tr_firca.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4974,11 +4980,11 @@
         <v>83</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>265</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gözlük','Initial','gözlük.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('g','gözlük','Initial','tr_gozluk.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4992,11 +4998,11 @@
         <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>220</v>
+        <v>167</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','hamur','Initial','hamur.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('h','hamur','Initial','tr_hamur.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5010,11 +5016,11 @@
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','kedi','Initial','kedi.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('k','kedi','Initial','tr_kedi.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5028,11 +5034,11 @@
         <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>169</v>
+        <v>222</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','lamba','Initial','lamba.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('l','lamba','Initial','tr_lamba.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5046,11 +5052,11 @@
         <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>223</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','makas','Initial','makas.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('m','makas','Initial','tr_makas.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5064,11 +5070,11 @@
         <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','nar','Initial','nar.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('n','nar','Initial','tr_nar.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -5082,11 +5088,11 @@
         <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','portakal','Initial','portakal.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('p','portakal','Initial','tr_portakal.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -5100,11 +5106,11 @@
         <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>172</v>
+        <v>225</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','resim','Initial','resim.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('r','resim','Initial','tr_resim.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -5118,11 +5124,11 @@
         <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>226</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','sabun','Initial','sabun.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('s','sabun','Initial','tr_sabun.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -5136,11 +5142,11 @@
         <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>174</v>
+        <v>258</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','şapka','Initial','şapka.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ş','şapka','Initial','tr_sapka.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5154,11 +5160,11 @@
         <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>175</v>
+        <v>227</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','tabak','Initial','tabak.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('t','tabak','Initial','tr_tabak.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5172,11 +5178,11 @@
         <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','vişne','Initial','vişne.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('v','vişne','Initial','tr_visne.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5190,11 +5196,11 @@
         <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yatak','Initial','yatak.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('y','yatak','Initial','tr_yatak.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5208,11 +5214,11 @@
         <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>229</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','zil','Initial','zil.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('z','zil','Initial','tr_zil.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5226,11 +5232,11 @@
         <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>230</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','kibrit','Medial','kibrit.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('b','kibrit','Medial','tr_kibrit.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5244,11 +5250,11 @@
         <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
+        <v>231</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('c','gece','Medial','gece.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('c','gece','Medial','tr_gece.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5262,11 +5268,11 @@
         <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>181</v>
+        <v>253</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','uçak','Medial','uçak.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ç','uçak','Medial','tr_ucak.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5280,11 +5286,11 @@
         <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>182</v>
+        <v>263</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','ördek','Medial','ördek.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('d','ördek','Medial','tr_ordek.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -5298,11 +5304,11 @@
         <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','köfte','Medial','köfte.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('f','köfte','Medial','tr_kofte.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5316,11 +5322,11 @@
         <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
+        <v>266</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','sünger','Medial','sünger.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('g','sünger','Medial','tr_sunger.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5334,11 +5340,11 @@
         <v>84</v>
       </c>
       <c r="D27" t="s">
-        <v>184</v>
+        <v>232</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','anahtar','Medial','anahtar.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('h','anahtar','Medial','tr_anahtar.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5352,11 +5358,11 @@
         <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>185</v>
+        <v>260</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','şeker','Medial','şeker.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('k','şeker','Medial','tr_seker.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -5370,11 +5376,11 @@
         <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>186</v>
+        <v>233</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','telefon','Medial','telefon.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('l','telefon','Medial','tr_telefon.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5388,11 +5394,11 @@
         <v>84</v>
       </c>
       <c r="D30" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','limon','Medial','limon.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('m','limon','Medial','tr_limon.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5406,11 +5412,11 @@
         <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>188</v>
+        <v>273</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','salıncak','Medial','salıncak.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('n','salıncak','Medial','tr_salincak.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -5424,11 +5430,11 @@
         <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>189</v>
+        <v>267</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','süpürge','Medial','süpürge.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('p','süpürge','Medial','tr_supurge.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -5442,11 +5448,11 @@
         <v>84</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>272</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','fırça','Medial','fırça.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('r','fırça','Medial','tr_firca.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5460,11 +5466,11 @@
         <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','taksi','Medial','taksi.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('s','taksi','Medial','tr_taksi.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -5478,11 +5484,11 @@
         <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>190</v>
+        <v>274</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','kaşık','Medial','kaşık.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ş','kaşık','Medial','tr_kasik.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -5496,11 +5502,11 @@
         <v>84</v>
       </c>
       <c r="D36" t="s">
-        <v>191</v>
+        <v>275</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','yastık','Medial','yastık.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('t','yastık','Medial','tr_yastik.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -5514,11 +5520,11 @@
         <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>192</v>
+        <v>261</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','tavşan','Medial','tavşan.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('v','tavşan','Medial','tr_tavsan.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -5532,11 +5538,11 @@
         <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','siyah','Medial','siyah.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('y','siyah','Medial','tr_siyah.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -5550,11 +5556,11 @@
         <v>84</v>
       </c>
       <c r="D39" t="s">
-        <v>194</v>
+        <v>268</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','üzüm','Medial','üzüm.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('z','üzüm','Medial','tr_uzum.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -5568,11 +5574,11 @@
         <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>195</v>
+        <v>254</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','havuç','Final','havuç.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ç','havuç','Final','tr_havuc.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -5586,11 +5592,11 @@
         <v>85</v>
       </c>
       <c r="D41" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','muz','Final','muz.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('f','muz','Final','tr_muz.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -5604,11 +5610,11 @@
         <v>85</v>
       </c>
       <c r="D42" t="s">
-        <v>196</v>
+        <v>236</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','puding','Final','puding.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('g','puding','Final','tr_puding.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -5622,11 +5628,11 @@
         <v>85</v>
       </c>
       <c r="D43" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('h','siyah','Final','siyah.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('h','siyah','Final','tr_siyah.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -5640,11 +5646,11 @@
         <v>85</v>
       </c>
       <c r="D44" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','park','Final','park.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('k','park','Final','tr_park.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -5658,11 +5664,11 @@
         <v>85</v>
       </c>
       <c r="D45" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','fil','Final','fil.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('l','fil','Final','tr_fil.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -5676,11 +5682,11 @@
         <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>239</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','kalem','Final','kalem.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('m','kalem','Final','tr_kalem.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -5694,11 +5700,11 @@
         <v>85</v>
       </c>
       <c r="D47" t="s">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','burun','Final','burun.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('n','burun','Final','tr_burun.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -5712,11 +5718,11 @@
         <v>85</v>
       </c>
       <c r="D48" t="s">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','kalp','Final','kalp.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('p','kalp','Final','tr_kalp.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -5730,11 +5736,11 @@
         <v>85</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','mantar','Final','mantar.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('r','mantar','Final','tr_mantar.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -5748,11 +5754,11 @@
         <v>85</v>
       </c>
       <c r="D50" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','dans','Final','dans.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('s','dans','Final','tr_dans.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -5766,11 +5772,11 @@
         <v>85</v>
       </c>
       <c r="D51" t="s">
-        <v>204</v>
+        <v>269</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','güneş','Final','güneş.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ş','güneş','Final','tr_gunes.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -5784,11 +5790,11 @@
         <v>85</v>
       </c>
       <c r="D52" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','at','Final','at.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('t','at','Final','tr_at.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -5802,11 +5808,11 @@
         <v>85</v>
       </c>
       <c r="D53" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','ev','Final','ev.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('v','ev','Final','tr_ev.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -5820,11 +5826,11 @@
         <v>85</v>
       </c>
       <c r="D54" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','çay','Final','çay.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('y','çay','Final','tr_cay.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -5838,11 +5844,11 @@
         <v>85</v>
       </c>
       <c r="D55" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','karpuz','Final','karpuz.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('z','karpuz','Final','tr_karpuz.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -5856,11 +5862,11 @@
         <v>86</v>
       </c>
       <c r="D56" t="s">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('b','bebek','Blended','bebek.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('b','bebek','Blended','tr_bebek.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -5874,11 +5880,11 @@
         <v>86</v>
       </c>
       <c r="D57" t="s">
-        <v>227</v>
+        <v>270</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('c','cüce','Blended','cüce.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('c','cüce','Blended','tr_cuce.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -5892,11 +5898,11 @@
         <v>86</v>
       </c>
       <c r="D58" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ç','çiçek','Blended','çiçek.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ç','çiçek','Blended','tr_cicek.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -5910,11 +5916,11 @@
         <v>86</v>
       </c>
       <c r="D59" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('d','dede','Blended','dede.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('d','dede','Blended','tr_dede.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -5928,11 +5934,11 @@
         <v>86</v>
       </c>
       <c r="D60" t="s">
-        <v>215</v>
+        <v>162</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('f','fotograf','Blended','fotograf.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('f','fotograf','Blended','tr_fotograf.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -5946,11 +5952,11 @@
         <v>86</v>
       </c>
       <c r="D61" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('g','gaga','Blended','gaga.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('g','gaga','Blended','tr_gaga.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -5964,11 +5970,11 @@
         <v>86</v>
       </c>
       <c r="D62" t="s">
-        <v>218</v>
+        <v>165</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('k','bakkal','Blended','bakkal.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('k','bakkal','Blended','tr_bakkal.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -5982,11 +5988,11 @@
         <v>86</v>
       </c>
       <c r="D63" t="s">
-        <v>222</v>
+        <v>169</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('l','lale','Blended','lale.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('l','lale','Blended','tr_lale.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -6000,11 +6006,11 @@
         <v>86</v>
       </c>
       <c r="D64" t="s">
-        <v>211</v>
+        <v>249</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('m','mum','Blended','mum.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('m','mum','Blended','tr_mum.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -6018,11 +6024,11 @@
         <v>86</v>
       </c>
       <c r="D65" t="s">
-        <v>217</v>
+        <v>164</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('n','ananas','Blended','ananas.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('n','ananas','Blended','tr_ananas.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -6036,11 +6042,11 @@
         <v>86</v>
       </c>
       <c r="D66" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('p','paspas','Blended','paspas.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('p','paspas','Blended','tr_paspas.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -6054,11 +6060,11 @@
         <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>213</v>
+        <v>271</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E73" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('",A67,"','",B67,"','",C67,"','",D67,"', 'TR');")</f>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('r','rüzgar','Blended','rüzgar.png', 'TR');</v>
+        <f t="shared" ref="E67:E73" si="1">CONCATENATE("INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('",A67,"','",B67,"','",C67,"','tr_",D67,"', 'TR',0);")</f>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('r','rüzgar','Blended','tr_ruzgar.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -6072,11 +6078,11 @@
         <v>86</v>
       </c>
       <c r="D68" t="s">
-        <v>225</v>
+        <v>172</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('s','seksen','Blended','seksen.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('s','seksen','Blended','tr_seksen.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -6090,11 +6096,11 @@
         <v>86</v>
       </c>
       <c r="D69" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('ş','şişman','Blended','şişman.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('ş','şişman','Blended','tr_sisman.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -6108,11 +6114,11 @@
         <v>86</v>
       </c>
       <c r="D70" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('t','tablet','Blended','tablet.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('t','tablet','Blended','tr_tablet.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -6126,11 +6132,11 @@
         <v>86</v>
       </c>
       <c r="D71" t="s">
-        <v>219</v>
+        <v>166</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('v','civciv','Blended','civciv.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('v','civciv','Blended','tr_civciv.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -6144,11 +6150,11 @@
         <v>86</v>
       </c>
       <c r="D72" t="s">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('y','yay','Blended','yay.png', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('y','yay','Blended','tr_yay.jpg', 'TR',0);</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -6162,11 +6168,11 @@
         <v>86</v>
       </c>
       <c r="D73" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode])  VALUES ('z','gazoz','Blended','gazoz.jpg', 'TR');</v>
+        <v>INSERT INTO [ArticulationTests] ([Sound],[Text],[SoundPosition],[Image], [LanguageCode], [Age])  VALUES ('z','gazoz','Blended','tr_gazoz.jpg', 'TR',0);</v>
       </c>
     </row>
   </sheetData>
@@ -6175,18 +6181,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD72"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" customWidth="1"/>
-    <col min="4" max="4" width="27.54296875" customWidth="1"/>
+    <col min="3" max="3" width="7.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6231,7 +6237,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
         <v>83</v>
@@ -6364,7 +6370,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>235</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
         <v>83</v>
@@ -6491,7 +6497,7 @@
         <v>157</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>240</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
         <v>83</v>
@@ -6567,7 +6573,7 @@
         <v>60</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>243</v>
+        <v>186</v>
       </c>
       <c r="C21" t="s">
         <v>83</v>
@@ -6583,10 +6589,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="22" t="s">
-        <v>244</v>
+        <v>187</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>245</v>
+        <v>188</v>
       </c>
       <c r="C22" t="s">
         <v>83</v>
@@ -6602,10 +6608,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="22" t="s">
-        <v>247</v>
+        <v>190</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>248</v>
+        <v>191</v>
       </c>
       <c r="C23" t="s">
         <v>83</v>
@@ -6675,7 +6681,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="C27" t="s">
         <v>84</v>
@@ -6897,7 +6903,7 @@
         <v>51</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>237</v>
+        <v>180</v>
       </c>
       <c r="C39" t="s">
         <v>84</v>
@@ -6916,7 +6922,7 @@
         <v>71</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>239</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
         <v>84</v>
@@ -6935,7 +6941,7 @@
         <v>157</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>241</v>
+        <v>184</v>
       </c>
       <c r="C41" t="s">
         <v>84</v>
@@ -7027,10 +7033,10 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="28" t="s">
-        <v>244</v>
+        <v>187</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>246</v>
+        <v>189</v>
       </c>
       <c r="C46" t="s">
         <v>84</v>
@@ -7046,7 +7052,7 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="28" t="s">
-        <v>247</v>
+        <v>190</v>
       </c>
       <c r="B47" s="29" t="s">
         <v>74</v>
@@ -7106,7 +7112,7 @@
         <v>5</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
       <c r="C50" t="s">
         <v>85</v>
@@ -7328,7 +7334,7 @@
         <v>57</v>
       </c>
       <c r="B62" s="29" t="s">
-        <v>236</v>
+        <v>179</v>
       </c>
       <c r="C62" t="s">
         <v>85</v>
@@ -7347,7 +7353,7 @@
         <v>51</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
         <v>85</v>
@@ -7385,7 +7391,7 @@
         <v>157</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>242</v>
+        <v>185</v>
       </c>
       <c r="C65" t="s">
         <v>85</v>
@@ -7477,7 +7483,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="28" t="s">
-        <v>244</v>
+        <v>187</v>
       </c>
       <c r="B70" s="29" t="s">
         <v>75</v>
@@ -7496,10 +7502,10 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="28" t="s">
-        <v>247</v>
+        <v>190</v>
       </c>
       <c r="B71" s="29" t="s">
-        <v>249</v>
+        <v>192</v>
       </c>
       <c r="C71" t="s">
         <v>85</v>
@@ -7551,14 +7557,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>